<commit_message>
done v1 flask app  prediksi
</commit_message>
<xml_diff>
--- a/triplet_output/test.xlsx
+++ b/triplet_output/test.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'benerin ', 'NEG')]</t>
+          <t>[('aplikasi', 'benerin', 'NEG')]</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -481,7 +481,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'rusak ', 'NEG'), ('aplikasi', 'ga niat ', 'NEG')]</t>
+          <t>[('aplikasi', 'rusak', 'NEG'), ('aplikasi', 'ga niat', 'NEG')]</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>[('sistem', 'eror ', 'NEG')]</t>
+          <t>[('sistem', 'eror', 'NEG')]</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>[('cari', 'ga muncul produknya ', 'NEG')]</t>
+          <t>[('cari produk', 'ga muncul produknya', 'NEG')]</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -541,7 +541,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sakti ', 'POS')]</t>
+          <t>[('aplikasi', 'sakti', 'POS')]</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'jlimet ', 'NEG')]</t>
+          <t>[('aplikasi', 'jlimet', 'NEG')]</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lemot sulit', 'NEG'), ('aplikasi', 'sulit masuk sih', 'NEG')]</t>
+          <t>[('aplikasi', 'lemot', 'NEG'), ('aplikasi', 'sulit masuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'kurang manfaat ', 'NEG'), ('pelayanan', 'sangat buruk ', 'NEG')]</t>
+          <t>[('aplikasi', 'kurang manfaat', 'NEG'), ('pelayanan', 'sangat buruk', 'NEG')]</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'hapuss ', 'NEG'), ('aplikasi', 'gak guna mending', 'NEG')]</t>
+          <t>[('aplikasi', 'hapuss', 'NEG'), ('aplikasi', 'gak guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -661,7 +661,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>[('didownload', 'ga bisa didownload', 'NEG')]</t>
+          <t>[('didownload', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -681,7 +681,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lawak ', 'NEG'), ('sertifikat', 'hilang semua', 'NEG')]</t>
+          <t>[('aplikasi', 'lawak', 'NEG'), ('sertifikat vaksin', 'hilang', 'NEG')]</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'meminimalkan mobilitas kita', 'POS'), ('aplikasi', 'memudahkan kita', 'POS')]</t>
+          <t>[('aplikasi', 'meminimalkan mobilitas', 'POS'), ('aplikasi', 'memudahkan', 'POS')]</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'payahnya minta ampun ', 'NEG')]</t>
+          <t>[('aplikasi', 'payahnya minta ampun', 'NEG')]</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -741,7 +741,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>[('server', 'tidak dapat terhubung ke', 'NEG')]</t>
+          <t>[('server', 'tidak dapat terhubung', 'NEG')]</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -761,7 +761,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>[('scan', 'tidak muncul tanggal', 'NEG')]</t>
+          <t>[('scan', 'tidak muncul', 'NEG')]</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>[('kualitas', 'sangat buriq ', 'NEG'), ('game', 'sangat buruk serta', 'NEG')]</t>
+          <t>[('kualitas grafiknya', 'sangat buriq', 'NEG'), ('game', 'sangat buruk', 'NEG')]</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'minta2 verifikasi ktp muka ', 'NEG'), ('aplikasi', 'minta2 indentitas ', 'NEG')]</t>
+          <t>[('aplikasi', 'minta2 verifikasi ktp muka', 'NEG'), ('aplikasi', 'minta2 indentitas', 'NEG')]</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -821,7 +821,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>[('masuk', 'susah ', 'NEG')]</t>
+          <t>[('masuk apk', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -841,7 +841,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>[('password', 'tulisannya bisa di munculin soalnya', 'NEG')]</t>
+          <t>[('password', 'tulisannya bisa di munculin', 'NEG')]</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -881,7 +881,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'senang ada', 'POS')]</t>
+          <t>[('pelayanan', 'senang', 'POS')]</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -901,7 +901,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'aneh ', 'NEG'), ('aplikasi', 'susah di gunakan ribet', 'NEG')]</t>
+          <t>[('aplikasi', 'aneh', 'NEG'), ('aplikasi', 'susah di gunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -921,7 +921,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ngk jelas ', 'NEG')]</t>
+          <t>[('aplikasi', 'ngk jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -941,7 +941,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>[('apk', 'gak bisa ', 'NEG')]</t>
+          <t>[('apk', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>[('biometrik', 'blum d atur ', 'POS')]</t>
+          <t>[('biometrik', 'blum d atur', 'POS')]</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'membantu dan', 'POS')]</t>
+          <t>[('aplikasi', 'membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>[('dftrnya', 'mudah df', 'POS')]</t>
+          <t>[('dftrnya', 'mudah', 'POS')]</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>[('login', 'sngat mudah ', 'POS')]</t>
+          <t>[('login', 'sngat mudah', 'POS')]</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1061,7 +1061,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'aneh ', 'NEG')]</t>
+          <t>[('aplikasinya', 'aneh', 'NEG')]</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1081,7 +1081,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>[('hasil', 'selalu memuaskan hasil', 'POS')]</t>
+          <t>[('hasil', 'selalu memuaskan', 'POS')]</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'sangat baik ', 'POS')]</t>
+          <t>[('pelayanan', 'sangat baik', 'POS')]</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1121,7 +1121,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>[('bug', 'cari bug', 'NEG')]</t>
+          <t>[('bug', 'cari', 'NEG')]</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1141,7 +1141,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>[('layanan', 'cepat sangat', 'POS')]</t>
+          <t>[('layanan', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -1161,7 +1161,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'cepat ', 'POS'), ('respon', 'cepat ', 'POS')]</t>
+          <t>[('pelayanan', 'cepat', 'POS'), ('respon', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>[('buka', 'tidak bisa di', 'NEG')]</t>
+          <t>[('buka', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1201,7 +1201,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak bisa di akses niat', 'NEG')]</t>
+          <t>[('aplikasi', 'gak bisa di akses', 'NEG')]</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gangguan kan', 'NEG')]</t>
+          <t>[('aplikasi', 'gangguan', 'NEG')]</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>[('update', 'tidak bekerja ', 'NEG'), ('update', 'tidak bekerja ', 'NEG')]</t>
+          <t>[('update tombol bookmarknya', 'tidak bekerja', 'NEG'), ('update', 'tidak bekerja', 'NEG')]</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>[('loading', 'ga berguna sama', 'NEG'), ('loading', 'lama bgt ', 'NEG')]</t>
+          <t>[('loading', 'ga berguna', 'NEG'), ('loading', 'lama bgt', 'NEG')]</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1301,7 +1301,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga guna ', 'NEG')]</t>
+          <t>[('aplikasi', 'ga guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1321,7 +1321,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>[('servernya', 'mati server', 'NEG')]</t>
+          <t>[('servernya', 'mati', 'NEG')]</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>[('server', 'ngga bisa terkoneksi dengan', 'NEG')]</t>
+          <t>[('server', 'ngga bisa terkoneksi', 'NEG')]</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'terbantu dengan', 'POS')]</t>
+          <t>[('aplikasi', 'terbantu', 'POS')]</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>[('app', 'sangat suka dengan', 'POS')]</t>
+          <t>[('app', 'sangat suka', 'POS')]</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -1401,7 +1401,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>[('responnya', 'cepet respon', 'POS')]</t>
+          <t>[('responnya', 'cepet', 'POS')]</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>[('menghemat', 'bisa menghemat', 'POS')]</t>
+          <t>[('menghemat waktu', 'bisa', 'POS')]</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -1441,7 +1441,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>[('login', 'susah bener', 'NEG'), ('aplikasi', 'gajelasssss login', 'NEG')]</t>
+          <t>[('login', 'susah', 'NEG'), ('aplikasi', 'gajelasssss', 'NEG')]</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat membantu ', 'POS')]</t>
+          <t>[('aplikasi', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'sangat membantu skali ', 'POS')]</t>
+          <t>[('pelayanan desa', 'sangat membantu skali', 'POS')]</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'busuk gaj', 'NEG'), ('aplikasi', 'busuk gajelas gab', 'NEG'), ('aplikasi', 'gabisa di gunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'busuk', 'NEG'), ('aplikasi', 'busuk gajelas', 'NEG'), ('aplikasi', 'gabisa di gunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -1521,7 +1521,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'g jelas ', 'NEG'), ('aplikasi', 'g guna ', 'NEG')]</t>
+          <t>[('aplikasi', 'g jelas', 'NEG'), ('aplikasi', 'g guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -1541,7 +1541,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>[('login', 'susah ', 'NEG')]</t>
+          <t>[('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -1561,7 +1561,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>[('dibuka', 'muter doang ', 'NEG'), ('ngecek', 'muter doang ', 'NEG')]</t>
+          <t>[('dibuka', 'muter doang', 'NEG'), ('ngecek', 'muter doang', 'NEG')]</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[('menu', 'tidak berfungsi ', 'NEG'), ('cek', 'susah ', 'NEG')]</t>
+          <t>[('menu', 'tidak berfungsi', 'NEG'), ('cek pajak kendaraan', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak guna ', 'NEG'), ('aplikasi', 'loading mulu ', 'NEG'), ('update', 'tidka update', 'NEG')]</t>
+          <t>[('aplikasi', 'gak guna', 'NEG'), ('aplikasi', 'loading mulu', 'NEG'), ('update', 'tidka', 'NEG')]</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -1621,7 +1621,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>[('cek', 'ga bs cek', 'NEG')]</t>
+          <t>[('cek nopol', 'ga bs', 'NEG')]</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>[('loginya', 'susah sekali login', 'NEG')]</t>
+          <t>[('loginya', 'susah sekali', 'NEG')]</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'terlantar ', 'NEG'), ('update', 'tidak ada update', 'NEG'), ('menu', 'hilang ', 'NEG'), ('update', 'tidak ada update', 'NEG')]</t>
+          <t>[('aplikasi', 'terlantar', 'NEG'), ('update aplikasi', 'tidak ada', 'NEG'), ('menu pembayaran', 'hilang', 'NEG'), ('update', 'tidak ada', 'NEG')]</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -1681,7 +1681,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>[('aplikasia', 'taekkk loading lama ', 'NEG')]</t>
+          <t>[('aplikasia', 'taekkk loading lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -1701,7 +1701,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>[('cek', 'gabisa cek', 'NEG')]</t>
+          <t>[('cek tnkb', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>[('daftar', 'sulit banget ', 'NEG')]</t>
+          <t>[('daftar', 'sulit banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>[('layanan', 'cepat ', 'POS'), ('layanan', 'sangat membantu ', 'POS')]</t>
+          <t>[('layanan', 'cepat', 'POS'), ('layanan', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>[('login', 'lamaa ', 'NEG'), ('login', 'ribett banget dan', 'NEG')]</t>
+          <t>[('login', 'lamaa', 'NEG'), ('login', 'ribett banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[('bug', 'masih banyak bug', 'NEG'), ('ui', 'perlu dirombak ', 'NEG')]</t>
+          <t>[('bug', 'masih banyak', 'NEG'), ('ui ux', 'perlu dirombak', 'NEG')]</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>[('pengaduan', 'cepat ', 'POS'), ('pengaduan', 'responsif ', 'POS')]</t>
+          <t>[('pengaduan', 'cepat', 'POS'), ('pengaduan', 'responsif', 'POS')]</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[('scan', 'kacau kadang', 'NEG'), ('aplikasi', 'lelet bgt aplikasi', 'NEG')]</t>
+          <t>[('scan barcode', 'kacau', 'NEG'), ('aplikasi', 'lelet bgt', 'NEG')]</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -1861,7 +1861,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bagus buat', 'POS')]</t>
+          <t>[('aplikasi', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -1881,7 +1881,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>[('respon', 'terlalu lama kurang', 'NEG')]</t>
+          <t>[('respon chat livenya', 'terlalu lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>[('ngecek', 'nggak bisa - bisa ', 'NEG'), ('aplikasi', 'payah ', 'NEG')]</t>
+          <t>[('ngecek pajak kendaraan', 'nggak bisa - bisa', 'NEG'), ('aplikasi', 'payah', 'NEG')]</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -1921,7 +1921,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak jelas ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -1941,7 +1941,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>[('cctv', 'ga bisa dibuka ', 'NEG')]</t>
+          <t>[('cctv', 'ga bisa dibuka', 'NEG')]</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -1961,7 +1961,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'eror mulu', 'NEG'), ('aplikasi', 'aneh eror', 'NEG')]</t>
+          <t>[('aplikasi', 'eror', 'NEG'), ('aplikasi', 'aneh', 'NEG')]</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>[('servernya', 'down ', 'NEG'), ('servernya', 'sering sekali server', 'NEG'), ('aplikasi', 'sering error ', 'NEG'), ('pelayanannya', 'tolong ditingkatkan lagi pelayanannya', 'NEG')]</t>
+          <t>[('servernya', 'down', 'NEG'), ('servernya', 'sering sekali', 'NEG'), ('aplikasi', 'sering error', 'NEG'), ('pelayanannya', 'tolong ditingkatkan lagi', 'NEG')]</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -2001,7 +2001,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>[('kartu', 'hilang ga', 'NEG')]</t>
+          <t>[('kartu vaksin', 'hilang', 'NEG')]</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -2021,7 +2021,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>[('infonya', 'kurang jelas dan', 'NEG'), ('infonya', 'kurang transparan ', 'NEG')]</t>
+          <t>[('infonya', 'kurang jelas', 'NEG'), ('infonya', 'kurang transparan', 'NEG')]</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -2041,7 +2041,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tambah ruwet ', 'NEG')]</t>
+          <t>[('aplikasi', 'tambah ruwet', 'NEG')]</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga jelas ', 'NEG'), ('aplikasinya', 'keluar sendiri aplikasinya', 'NEG')]</t>
+          <t>[('aplikasi', 'ga jelas', 'NEG'), ('aplikasinya', 'keluar sendiri', 'NEG')]</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'praktis ', 'POS'), ('responnya', 'cepat juga', 'POS'), ('verifikasinya', 'cepat ', 'POS')]</t>
+          <t>[('aplikasi', 'praktis', 'POS'), ('responnya', 'cepat', 'POS'), ('verifikasinya', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>[('landscape', 'gabisa land', 'NEG')]</t>
+          <t>[('landscape', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>[('dibuka', 'ga bisa dibuka', 'NEG')]</t>
+          <t>[('dibuka', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>[('apk', 'tidak berguna ', 'NEG')]</t>
+          <t>[('apk', 'tidak berguna', 'NEG')]</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>[('daftar', 'tidak bisa daftar', 'NEG')]</t>
+          <t>[('daftar kurma', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>[('data', 'kurang akurat ', 'NEG')]</t>
+          <t>[('data', 'kurang akurat', 'NEG')]</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -2201,7 +2201,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bnyk bug ', 'NEG'), ('apk', 'membingungkan ', 'NEG')]</t>
+          <t>[('aplikasi', 'bnyk bug', 'NEG'), ('apk', 'membingungkan', 'NEG')]</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -2221,7 +2221,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>[('akses', 'mempermudah untuk', 'POS')]</t>
+          <t>[('akses data', 'mempermudah', 'POS')]</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -2241,7 +2241,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tdk dikelola dg', 'NEG'), ('scan', 'lama ', 'NEG')]</t>
+          <t>[('aplikasi', 'tdk dikelola', 'NEG'), ('scan qr', 'lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -2261,7 +2261,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>[('bookmark', 'tidak bisa bookmark', 'NEG')]</t>
+          <t>[('bookmark', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -2281,7 +2281,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>[('ganguan', 'banyak gang', 'NEG')]</t>
+          <t>[('ganguan', 'banyak', 'NEG')]</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -2301,7 +2301,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>[('info', 'segera diakses oleh', 'POS'), ('aplikasi', 'lengkap ', 'POS'), ('aplikasi', 'mudah digunakan ', 'POS'), ('aplikasi', 'cepat ', 'POS')]</t>
+          <t>[('info terkini', 'segera diakses', 'POS'), ('aplikasi', 'lengkap', 'POS'), ('aplikasi', 'mudah digunakan', 'POS'), ('aplikasi', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lebih simpel pake', 'POS')]</t>
+          <t>[('aplikasi', 'lebih simpel', 'POS')]</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>[('apl', 'tidak membantu sama', 'NEG')]</t>
+          <t>[('apl', 'tidak membantu', 'NEG')]</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -2361,7 +2361,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga guna ', 'NEG')]</t>
+          <t>[('aplikasi', 'ga guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -2381,7 +2381,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'ga bisa digunakan buat ngecek nop', 'NEG')]</t>
+          <t>[('aplikasinya', 'ga bisa digunakan buat ngecek', 'NEG')]</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -2421,7 +2421,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>[('scan', 'terlalu lama mendeteksinya ', 'NEG')]</t>
+          <t>[('scan barcodenya', 'terlalu lama mendeteksinya', 'NEG')]</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -2461,7 +2461,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>[('bikin', 'ribet ', 'NEG'), ('email', 'tak dpat balasan dr', 'NEG')]</t>
+          <t>[('bikin surat kelahiran', 'ribet', 'NEG'), ('email', 'tak dpat balasan', 'NEG')]</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -2481,7 +2481,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>[('ngecek', 'gak bisa ngec', 'NEG'), ('tampilan', 'beda jadi', 'NEG')]</t>
+          <t>[('ngecek', 'gak bisa', 'NEG'), ('tampilan', 'beda', 'NEG')]</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>[('server', 'gk bisa masuk k', 'NEG')]</t>
+          <t>[('server', 'gk bisa masuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>[('scan', 'ga bisa ', 'NEG'), ('unduh', 'ga bisa unduh', 'NEG')]</t>
+          <t>[('scan barcode', 'ga bisa', 'NEG'), ('unduh sertif', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -2541,7 +2541,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'membantu sekali aplikasi', 'POS')]</t>
+          <t>[('aplikasi', 'membantu sekali', 'POS')]</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -2561,7 +2561,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>[('cek', 'tidak ada ', 'NEG')]</t>
+          <t>[('cek hasil', 'tidak ada', 'NEG')]</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>[('cek', 'tidak bisa untuk', 'NEG')]</t>
+          <t>[('cek', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -2601,7 +2601,7 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>[('tombolnya', 'gak fungsi ', 'NEG')]</t>
+          <t>[('tombolnya', 'gak fungsi', 'NEG')]</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>[('login', 'tidak bisa login', 'NEG')]</t>
+          <t>[('login', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
@@ -2641,7 +2641,7 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>[('scan', 'muter terus sampe', 'NEG'), ('aplikasi', 'goblog scan', 'NEG')]</t>
+          <t>[('scan barcode', 'muter terus', 'NEG'), ('aplikasi', 'goblog', 'NEG')]</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'cepat ', 'POS')]</t>
+          <t>[('pelayanan', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -2681,7 +2681,7 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak bisa di buka ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak bisa di buka', 'NEG')]</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>[('pengurusan', 'sangatlah mudah dengan', 'POS')]</t>
+          <t>[('pengurusan dokumen', 'sangatlah mudah', 'POS')]</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>[('scan', 'tidak bisa fokus akhirnya', 'NEG'), ('aplikasinya', 'bagus sy', 'POS')]</t>
+          <t>[('scan barcodenya', 'tidak bisa fokus', 'NEG'), ('aplikasinya', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
@@ -2741,7 +2741,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>[('pake', 'ga bisa di', 'NEG')]</t>
+          <t>[('pake', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -2781,7 +2781,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>[('mencari', 'sangat memudahkan kita', 'POS')]</t>
+          <t>[('mencari buku bacaan', 'sangat memudahkan', 'POS')]</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>[('masuk', 'banya problem buat', 'NEG')]</t>
+          <t>[('masuk', 'banya problem', 'NEG')]</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -2821,7 +2821,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>[('aktivasinya', 'gk di kirim2 ke', 'NEG')]</t>
+          <t>[('aktivasinya', 'gk di kirim2', 'NEG')]</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -2841,7 +2841,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'keluar aplikasi', 'NEG')]</t>
+          <t>[('aplikasi', 'keluar', 'NEG')]</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -2861,7 +2861,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>[('application', 'bad application', 'NEG')]</t>
+          <t>[('application', 'bad', 'NEG')]</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -2901,7 +2901,7 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>[('scan', 'gbs di', 'NEG')]</t>
+          <t>[('scan', 'gbs', 'NEG')]</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -2921,7 +2921,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>[('fitur', 'makin jelek fitur', 'NEG')]</t>
+          <t>[('fitur layanan aplikasi', 'makin jelek', 'NEG')]</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>[('loading', 'ga kelar ga', 'NEG'), ('loading', 'mulu ga', 'NEG'), ('loading', 'ga kelar ga kelacak ', 'NEG')]</t>
+          <t>[('loading', 'ga kelar', 'NEG'), ('loading', 'mulu', 'NEG'), ('loading', 'ga kelar ga kelacak', 'NEG')]</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -2961,7 +2961,7 @@
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'lemot sye', 'NEG')]</t>
+          <t>[('aplikasinya', 'lemot', 'NEG')]</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -2981,7 +2981,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>[('cek', 'error bug', 'NEG'), ('aplikasi', 'sering log out sendiri ', 'NEG')]</t>
+          <t>[('cek aplikasi', 'error', 'NEG'), ('aplikasi', 'sering log out sendiri', 'NEG')]</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -3001,7 +3001,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>[('web', 'tidak bisa diakses ', 'NEG'), ('update', 'tidak bisa diakses ', 'NEG')]</t>
+          <t>[('web', 'tidak bisa diakses', 'NEG'), ('update', 'tidak bisa diakses', 'NEG')]</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga berguna ', 'NEG')]</t>
+          <t>[('aplikasi', 'ga berguna', 'NEG')]</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'sangat perlu diperbaiki aplikasinya', 'NEG')]</t>
+          <t>[('aplikasinya', 'sangat perlu diperbaiki', 'NEG')]</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -3061,7 +3061,7 @@
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>[('daftar', 'tidak bisa daftar', 'NEG')]</t>
+          <t>[('daftar', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'aneh banyak', 'NEG')]</t>
+          <t>[('aplikasi', 'aneh', 'NEG')]</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>[('diakses', 'ga bisa diakses', 'NEG')]</t>
+          <t>[('diakses', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>[('kinerja', 'sangat responsif &amp;', 'POS')]</t>
+          <t>[('kinerja jaki', 'sangat responsif', 'POS')]</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -3161,7 +3161,7 @@
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>[('server', 'ga jelas gimana', 'NEG')]</t>
+          <t>[('server', 'ga jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>[('servee', 'ga konek serv', 'NEG')]</t>
+          <t>[('servee', 'ga konek', 'NEG')]</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -3201,7 +3201,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>[('aolikasi', 'errorr mulu', 'NEG')]</t>
+          <t>[('aolikasi', 'errorr', 'NEG')]</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -3221,7 +3221,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>[('cek', 'tidak dapat cek', 'NEG')]</t>
+          <t>[('cek pajak kendaraan', 'tidak dapat', 'NEG')]</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>[('kirim', 'gak masuk2 sampe', 'NEG')]</t>
+          <t>[('kirim kode verifikasi', 'gak masuk2', 'NEG')]</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>[('pelatanannya', 'sangat memuaskan ', 'POS')]</t>
+          <t>[('pelatanannya', 'sangat memuaskan', 'POS')]</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -3301,7 +3301,7 @@
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>[('masuk', 'mental terus ', 'NEG')]</t>
+          <t>[('masuk wifi', 'mental terus', 'NEG')]</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>[('plat', 'tidak terdeteksi ', 'NEG'), ('aplikasi', 'gak bisa digunakan ', 'NEG')]</t>
+          <t>[('plat nomor', 'tidak terdeteksi', 'NEG'), ('aplikasi', 'gak bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -3381,7 +3381,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>[('update', 'mandek ditengah', 'NEG')]</t>
+          <t>[('update', 'mandek', 'NEG')]</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga guna dari', 'NEG')]</t>
+          <t>[('aplikasi', 'ga guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -3421,7 +3421,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>[('cek', 'ga bisa cek', 'NEG')]</t>
+          <t>[('cek pajak', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -3441,7 +3441,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>[('tes', 'susah ', 'NEG'), ('aplikasi', 'rusak ', 'NEG')]</t>
+          <t>[('tes', 'susah', 'NEG'), ('aplikasi', 'rusak', 'NEG')]</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -3461,7 +3461,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>[('download', 'ga bisa ya', 'NEG')]</t>
+          <t>[('download sertifikat vaksin', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>[('diupdate', 'makin eror ', 'NEG')]</t>
+          <t>[('diupdate', 'makin eror', 'NEG')]</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'tidak dapat mengakses aplikasinya', 'NEG'), ('login', '" tidak dapat terkoneksi ke', 'NEG'), ('login', 'gabisa ', 'NEG'), ('server', '" tidak dapat terkoneksi ke', 'NEG')]</t>
+          <t>[('aplikasinya', 'tidak dapat mengakses', 'NEG'), ('login', '" tidak dapat terkoneksi', 'NEG'), ('login', 'gabisa', 'NEG'), ('server "', '" tidak dapat terkoneksi', 'NEG')]</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
@@ -3521,7 +3521,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>[('login', 'ga bisa login', 'NEG')]</t>
+          <t>[('login', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
@@ -3541,7 +3541,7 @@
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>[('cek', 'gak bisa ', 'NEG')]</t>
+          <t>[('cek pajak kendaraan', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bagus ', 'POS')]</t>
+          <t>[('aplikasi', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
@@ -3581,7 +3581,7 @@
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'makin gak jelas ini', 'NEG')]</t>
+          <t>[('aplikasi', 'makin gak jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
@@ -3601,7 +3601,7 @@
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>[('buka', 'tidak bisa di', 'NEG')]</t>
+          <t>[('buka', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
@@ -3621,7 +3621,7 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>[('notifikasi', 'gak muncul di', 'NEG')]</t>
+          <t>[('notifikasi ketersediaan buku', 'gak muncul', 'NEG')]</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>[('adminduk', 'memudahkan warga', 'POS'), ('pengurusan', 'memudahkan warga', 'POS')]</t>
+          <t>[('adminduk', 'memudahkan', 'POS'), ('pengurusan adminduk', 'memudahkan', 'POS')]</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
@@ -3661,7 +3661,7 @@
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>[('loading', 'ga jelas ', 'NEG')]</t>
+          <t>[('loading', 'ga jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
@@ -3681,7 +3681,7 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>[('cek', 'gak bisa ', 'NEG')]</t>
+          <t>[('cek pajak', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
@@ -3701,7 +3701,7 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'mantep ', 'POS')]</t>
+          <t>[('pelayanan', 'mantep', 'POS')]</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>[('apk', 'gak pakai apk', 'NEG')]</t>
+          <t>[('apk', 'gak pakai', 'NEG')]</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
@@ -3741,7 +3741,7 @@
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>[('kode', 'gk ada data ', 'NEG')]</t>
+          <t>[('kode', 'gk ada data', 'NEG')]</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
@@ -3761,7 +3761,7 @@
       </c>
       <c r="C167" t="inlineStr">
         <is>
-          <t>[('login', 'susah nya', 'NEG')]</t>
+          <t>[('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>[('exp', 'tidak bisa mengecek exp', 'NEG')]</t>
+          <t>[('exp produk', 'tidak bisa mengecek', 'NEG')]</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
@@ -3801,7 +3801,7 @@
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>[('pemeliharaan', 'disepelekan pemeliharaan', 'NEG')]</t>
+          <t>[('pemeliharaan', 'disepelekan', 'NEG')]</t>
         </is>
       </c>
       <c r="D169" t="inlineStr">
@@ -3821,7 +3821,7 @@
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat bangga dengan', 'POS')]</t>
+          <t>[('aplikasi', 'sangat bangga', 'POS')]</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
@@ -3841,7 +3841,7 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak berguna ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak berguna', 'NEG')]</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>[('kode', 'busuk ', 'NEG')]</t>
+          <t>[('kode otp', 'busuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
@@ -3881,7 +3881,7 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>[('ikon', 'ga ada ikon', 'NEG')]</t>
+          <t>[('ikon', 'ga ada', 'NEG')]</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
@@ -3901,7 +3901,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>[('scan', 'lama banget ', 'NEG')]</t>
+          <t>[('scan', 'lama banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
@@ -3921,7 +3921,7 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>[('laporan', 'langsung ditanggapi ', 'POS')]</t>
+          <t>[('laporan', 'langsung ditanggapi', 'POS')]</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>[('scan', 'buram tp', 'NEG')]</t>
+          <t>[('scan gambarnya', 'buram', 'NEG')]</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
@@ -3961,7 +3961,7 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ngontol ', 'NEG'), ('loginnya', 'ribet banget login', 'NEG')]</t>
+          <t>[('aplikasi', 'ngontol', 'NEG'), ('loginnya', 'ribet banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
@@ -3981,7 +3981,7 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>[('liat', 'gabisa liat', 'NEG')]</t>
+          <t>[('liat sertifikat vaksin', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
@@ -4001,7 +4001,7 @@
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak bisa digunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lemot biang', 'NEG')]</t>
+          <t>[('aplikasi', 'lemot', 'NEG')]</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -4041,7 +4041,7 @@
       </c>
       <c r="C181" t="inlineStr">
         <is>
-          <t>[('qr', 'kaga bisa q', 'NEG')]</t>
+          <t>[('qr', 'kaga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D181" t="inlineStr">
@@ -4061,7 +4061,7 @@
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>[('apk', 'ampe kiamat , yg shrusnya apk', 'NEG'), ('scan', 'ampe kiamat ', 'NEG')]</t>
+          <t>[('apk', 'ampe kiamat , yg shrusnya', 'NEG'), ('scan', 'ampe kiamat', 'NEG')]</t>
         </is>
       </c>
       <c r="D182" t="inlineStr">
@@ -4081,7 +4081,7 @@
       </c>
       <c r="C183" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sampah ', 'NEG'), ('masuk', 'gak bisa masuk', 'NEG')]</t>
+          <t>[('aplikasi', 'sampah', 'NEG'), ('masuk', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D183" t="inlineStr">
@@ -4101,7 +4101,7 @@
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ribet ', 'NEG')]</t>
+          <t>[('aplikasi', 'ribet', 'NEG')]</t>
         </is>
       </c>
       <c r="D184" t="inlineStr">
@@ -4121,7 +4121,7 @@
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lama sekali padahal', 'NEG'), ('download', 'lama sekali padahal', 'NEG')]</t>
+          <t>[('aplikasi', 'lama sekali', 'NEG'), ('download aplikasi', 'lama sekali', 'NEG')]</t>
         </is>
       </c>
       <c r="D185" t="inlineStr">
@@ -4141,7 +4141,7 @@
       </c>
       <c r="C186" t="inlineStr">
         <is>
-          <t>[('ngedeteksi', 'cepet pula', 'POS')]</t>
+          <t>[('ngedeteksi', 'cepet', 'POS')]</t>
         </is>
       </c>
       <c r="D186" t="inlineStr">
@@ -4161,7 +4161,7 @@
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sagat berat ', 'NEG'), ('aplikasi', 'selalu loading terus', 'NEG')]</t>
+          <t>[('aplikasi', 'sagat berat', 'NEG'), ('aplikasi', 'selalu loading', 'NEG')]</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -4181,7 +4181,7 @@
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>[('ganti', 'ribet ', 'NEG')]</t>
+          <t>[('ganti pin', 'ribet', 'NEG')]</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
@@ -4201,7 +4201,7 @@
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat membantu dari', 'POS')]</t>
+          <t>[('aplikasi', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -4221,7 +4221,7 @@
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>[('upgrade', 'gk bisa buat', 'NEG'), ('ngecek', 'gk bisa buat', 'NEG')]</t>
+          <t>[('upgrade', 'gk bisa', 'NEG'), ('ngecek', 'gk bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>[('penanganan', 'cepat tapi', 'POS'), ('penanganan', 'tingkatkan lagi biar', 'POS')]</t>
+          <t>[('penanganan', 'cepat', 'POS'), ('penanganan', 'tingkatkan lagi', 'POS')]</t>
         </is>
       </c>
       <c r="D191" t="inlineStr">
@@ -4261,7 +4261,7 @@
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>[('ngurus', 'dipersulit sebenernya', 'NEG')]</t>
+          <t>[('ngurus surat kematian', 'dipersulit', 'NEG')]</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -4281,7 +4281,7 @@
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>[('login', 'gabisa login', 'NEG')]</t>
+          <t>[('login', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -4301,7 +4301,7 @@
       </c>
       <c r="C194" t="inlineStr">
         <is>
-          <t>[('kode', 'ga dikssih2 ki', 'NEG')]</t>
+          <t>[('kode aktivasi', 'ga dikssih2', 'NEG')]</t>
         </is>
       </c>
       <c r="D194" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>[('pakai', 'gak bisa di', 'NEG')]</t>
+          <t>[('pakai', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D195" t="inlineStr">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>[('tanggapan', 'cepat gx', 'POS')]</t>
+          <t>[('tanggapan', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D196" t="inlineStr">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="C197" t="inlineStr">
         <is>
-          <t>[('scan', 'tak bisa scan', 'NEG'), ('dipakai', 'tidak bisa dipakai', 'NEG')]</t>
+          <t>[('scan', 'tak bisa', 'NEG'), ('dipakai', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D197" t="inlineStr">
@@ -4381,7 +4381,7 @@
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'bagus ', 'POS')]</t>
+          <t>[('pelayanan disdukcapil', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D198" t="inlineStr">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'baik tp', 'NEG'), ('server', 'buruk ', 'NEG')]</t>
+          <t>[('aplikasi', 'baik', 'NEG'), ('server', 'buruk', 'NEG')]</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -4421,7 +4421,7 @@
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat jelek ', 'NEG')]</t>
+          <t>[('aplikasi', 'sangat jelek', 'NEG')]</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -4441,7 +4441,7 @@
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>[('apk', 'nyebelin banget apk', 'NEG')]</t>
+          <t>[('apk', 'nyebelin banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -4461,7 +4461,7 @@
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>[('update', 'ga bisa di pakai ', 'NEG')]</t>
+          <t>[('update', 'ga bisa di pakai', 'NEG')]</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gk jelas ', 'NEG')]</t>
+          <t>[('aplikasi', 'gk jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -4501,7 +4501,7 @@
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak dapat terkoneksi ke internet ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak dapat terkoneksi ke internet', 'NEG')]</t>
         </is>
       </c>
       <c r="D204" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tolol ', 'NEG')]</t>
+          <t>[('aplikasi', 'tolol', 'NEG')]</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="C207" t="inlineStr">
         <is>
-          <t>[('apl', 'eror eror', 'NEG')]</t>
+          <t>[('apl', 'eror', 'NEG')]</t>
         </is>
       </c>
       <c r="D207" t="inlineStr">
@@ -4581,7 +4581,7 @@
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>[('login', 'gabisa padahal', 'NEG'), ('aplikasi', 'tolong diperbaiki ini', 'NEG'), ('aplikasi', 'lemott ', 'NEG'), ('cek', 'lemott ', 'NEG')]</t>
+          <t>[('login', 'gabisa', 'NEG'), ('aplikasi', 'tolong diperbaiki', 'NEG'), ('aplikasi', 'lemott', 'NEG'), ('cek obat yang banyak bgt aplikasi', 'lemott', 'NEG')]</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="C209" t="inlineStr">
         <is>
-          <t>[('penggunaannya', 'susah penggunaannya', 'NEG')]</t>
+          <t>[('penggunaannya', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D209" t="inlineStr">
@@ -4621,7 +4621,7 @@
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>[('cek', 'tidak bisa cek', 'NEG')]</t>
+          <t>[('cek pajak kendaraan', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -4641,7 +4641,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>[('cek', 'loading lama ', 'NEG')]</t>
+          <t>[('cek prodak', 'loading lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D211" t="inlineStr">
@@ -4661,7 +4661,7 @@
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>[('apknya', 'jelek ', 'NEG'), ('verifikasi', 'gak masuk gad', 'NEG')]</t>
+          <t>[('apknya', 'jelek', 'NEG'), ('verifikasi email', 'gak masuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -4701,7 +4701,7 @@
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'belum siap ', 'NEG'), ('respon', 'tidak ada', 'NEG')]</t>
+          <t>[('aplikasi', 'belum siap', 'NEG'), ('respon', 'tidak', 'NEG')]</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -4721,7 +4721,7 @@
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bodoh ', 'NEG'), ('aplikasi', 'gak jelaps ', 'NEG'), ('iklan', 'susah masuk ', 'NEG')]</t>
+          <t>[('aplikasi', 'bodoh', 'NEG'), ('aplikasi', 'gak jelaps', 'NEG'), ('iklan', 'susah masuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
@@ -4741,7 +4741,7 @@
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak bisa submit laporan ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak bisa submit laporan', 'NEG')]</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -4761,7 +4761,7 @@
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>[('lupa', 'tidak ada ', 'NEG')]</t>
+          <t>[('lupa pasword', 'tidak ada', 'NEG')]</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>[('applikasi', 'tidak bisa dibuka ', 'NEG'), ('applikasi', 'gak bisa dibuka juga', 'NEG')]</t>
+          <t>[('applikasi', 'tidak bisa dibuka', 'NEG'), ('applikasi', 'gak bisa dibuka', 'NEG')]</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -4801,7 +4801,7 @@
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>[('admin', 'mantaaap admin', 'POS'), ('admin', 'gercep banget ', 'NEG')]</t>
+          <t>[('admin', 'mantaaap', 'POS'), ('admin', 'gercep banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D219" t="inlineStr">
@@ -4821,7 +4821,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>[('login', 'lama sekali ', 'NEG'), ('logging', 'belum bisa log', 'NEG'), ('logging', 'lambat ', 'NEG')]</t>
+          <t>[('login', 'lama sekali', 'NEG'), ('logging in', 'belum bisa', 'NEG'), ('logging in', 'lambat', 'NEG')]</t>
         </is>
       </c>
       <c r="D220" t="inlineStr">
@@ -4841,7 +4841,7 @@
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tolol ini', 'NEG')]</t>
+          <t>[('aplikasi', 'tolol', 'NEG')]</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>[('pembayaran', 'cukup membantu untuk', 'POS')]</t>
+          <t>[('pembayaran pajak bermotor', 'cukup membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -4881,7 +4881,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tolol hapus', 'NEG'), ('apk', 'sampah gag', 'NEG')]</t>
+          <t>[('aplikasi', 'tolol', 'NEG'), ('apk', 'sampah', 'NEG')]</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
@@ -4901,7 +4901,7 @@
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>[('update', 'brsan update', 'NEG')]</t>
+          <t>[('update', 'brsan', 'NEG')]</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>[('registrasi', 'susah ', 'NEG')]</t>
+          <t>[('registrasi', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'cepat ', 'POS'), ('pelayanan', 'bagus dan', 'POS')]</t>
+          <t>[('pelayanan', 'cepat', 'POS'), ('pelayanan', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D226" t="inlineStr">
@@ -4961,7 +4961,7 @@
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>[('apknya', 'perbaiki apk', 'NEG'), ('masuk', 'tidak bisa masuk', 'NEG')]</t>
+          <t>[('apknya', 'perbaiki', 'NEG'), ('masuk', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D227" t="inlineStr">
@@ -4981,7 +4981,7 @@
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'belum beres ', 'NEG')]</t>
+          <t>[('aplikasi', 'belum beres', 'NEG')]</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
@@ -5001,7 +5001,7 @@
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat bermanfaat bagi', 'POS')]</t>
+          <t>[('aplikasi', 'sangat bermanfaat', 'POS')]</t>
         </is>
       </c>
       <c r="D229" t="inlineStr">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'sangat bermanfaat ', 'POS')]</t>
+          <t>[('aplikasinya', 'sangat bermanfaat', 'POS')]</t>
         </is>
       </c>
       <c r="D230" t="inlineStr">
@@ -5041,7 +5041,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gajelas ', 'NEG')]</t>
+          <t>[('aplikasi', 'gajelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D231" t="inlineStr">
@@ -5061,7 +5061,7 @@
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>[('buka', 'susah di', 'NEG')]</t>
+          <t>[('buka', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>[('masuk', 'susah apalagi', 'NEG')]</t>
+          <t>[('masuk', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D233" t="inlineStr">
@@ -5101,7 +5101,7 @@
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>[('ngecek', 'susah ', 'NEG')]</t>
+          <t>[('ngecek pembayaran', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D234" t="inlineStr">
@@ -5121,7 +5121,7 @@
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>[('ngurus', 'susahnya minta ampun ', 'NEG')]</t>
+          <t>[('ngurus dokumen', 'susahnya minta ampun', 'NEG')]</t>
         </is>
       </c>
       <c r="D235" t="inlineStr">
@@ -5141,7 +5141,7 @@
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak bisa digunakan ', 'NEG'), ('aplikasi', 'tolong diperbaiki segera', 'NEG'), ('alat', 'tidak berfungsi sebagaimana', 'NEG'), ('scan', 'tidak berfungsi sebagaimana', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak bisa digunakan', 'NEG'), ('aplikasi', 'tolong diperbaiki', 'NEG'), ('alat scan', 'tidak berfungsi', 'NEG'), ('scan', 'tidak berfungsi', 'NEG')]</t>
         </is>
       </c>
       <c r="D236" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>[('log', 'gak bisa log', 'NEG')]</t>
+          <t>[('log in', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D237" t="inlineStr">
@@ -5181,7 +5181,7 @@
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>[('aplikasinys', 'tidak bisa ', 'NEG')]</t>
+          <t>[('aplikasinys', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -5201,7 +5201,7 @@
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>[('scan', 'gak bisa di gunakan sama', 'NEG'), ('fitur', 'gak bisa di gunakan sama', 'NEG')]</t>
+          <t>[('scan barcodenya', 'gak bisa di gunakan', 'NEG'), ('fitur scan barcodenya', 'gak bisa di gunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D239" t="inlineStr">
@@ -5221,7 +5221,7 @@
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>[('login', 'susah banget mau', 'NEG'), ('login', 'gagal mulu dan', 'NEG')]</t>
+          <t>[('login', 'susah banget', 'NEG'), ('login', 'gagal mulu', 'NEG')]</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -5241,7 +5241,7 @@
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>[('ganti', 'gabisa ganti', 'NEG')]</t>
+          <t>[('ganti email', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>[('cek', 'ga bisa cek', 'NEG'), ('cek', 'error ', 'NEG')]</t>
+          <t>[('cek plat', 'ga bisa', 'NEG'), ('cek plat', 'error', 'NEG')]</t>
         </is>
       </c>
       <c r="D242" t="inlineStr">
@@ -5281,7 +5281,7 @@
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>[('hotspot', 'nggak bisa dipakek ', 'NEG')]</t>
+          <t>[('hotspot', 'nggak bisa dipakek', 'NEG')]</t>
         </is>
       </c>
       <c r="D243" t="inlineStr">
@@ -5301,7 +5301,7 @@
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'memuaskan ', 'POS'), ('pelayanan', 'sangat bagus dan', 'POS')]</t>
+          <t>[('pelayanan', 'memuaskan', 'POS'), ('pelayanan', 'sangat bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D244" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'jelek gak', 'NEG'), ('aplikasi', 'gak bisa cek ', 'NEG')]</t>
+          <t>[('aplikasi', 'jelek', 'NEG'), ('aplikasi', 'gak bisa cek', 'NEG')]</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -5341,7 +5341,7 @@
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>[('login2', 'nggak bisa di', 'NEG')]</t>
+          <t>[('login2', 'nggak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D246" t="inlineStr">
@@ -5361,7 +5361,7 @@
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>[('loading', 'terusss baru', 'NEG')]</t>
+          <t>[('loading', 'terusss', 'NEG')]</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -5381,7 +5381,7 @@
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>[('server', 'tidak terkoneksi ke', 'NEG')]</t>
+          <t>[('server', 'tidak terkoneksi', 'NEG')]</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
@@ -5401,7 +5401,7 @@
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'jelek mau', 'NEG')]</t>
+          <t>[('aplikasi', 'jelek', 'NEG')]</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
@@ -5421,7 +5421,7 @@
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>[('daftar', 'ga bs ', 'NEG')]</t>
+          <t>[('daftar', 'ga bs', 'NEG')]</t>
         </is>
       </c>
       <c r="D250" t="inlineStr">
@@ -5441,7 +5441,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'sangat memuaskan ', 'POS')]</t>
+          <t>[('pelayanan', 'sangat memuaskan', 'POS')]</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>[('update', 'nggak fungsi ', 'NEG')]</t>
+          <t>[('update', 'nggak fungsi', 'NEG')]</t>
         </is>
       </c>
       <c r="D252" t="inlineStr">
@@ -5481,7 +5481,7 @@
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>[('apk', 'goks ', 'NEG')]</t>
+          <t>[('apk', 'goks', 'NEG')]</t>
         </is>
       </c>
       <c r="D253" t="inlineStr">
@@ -5501,7 +5501,7 @@
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>[('fiturnya', 'semakin lengkap fitur', 'POS')]</t>
+          <t>[('fiturnya', 'semakin lengkap', 'POS')]</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
@@ -5521,7 +5521,7 @@
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'sangat membantu dengan', 'POS')]</t>
+          <t>[('pelayanan', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'cepat dan', 'POS'), ('pelayanan', 'tydak ribet ', 'NEG')]</t>
+          <t>[('pelayanan', 'cepat', 'POS'), ('pelayanan', 'tydak ribet', 'NEG')]</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga bisa di gunain si', 'NEG')]</t>
+          <t>[('aplikasi', 'ga bisa di gunain', 'NEG')]</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
@@ -5581,7 +5581,7 @@
       </c>
       <c r="C258" t="inlineStr">
         <is>
-          <t>[('apli', 'nggak jelas dan', 'NEG'), ('apli', 'menyita waktu ', 'NEG')]</t>
+          <t>[('apli', 'nggak jelas', 'NEG'), ('apli', 'menyita waktu', 'NEG')]</t>
         </is>
       </c>
       <c r="D258" t="inlineStr">
@@ -5601,7 +5601,7 @@
       </c>
       <c r="C259" t="inlineStr">
         <is>
-          <t>[('scan', 'nggak bisa untuk', 'NEG'), ('loading', 'lama banget dan', 'NEG')]</t>
+          <t>[('scan produk', 'nggak bisa', 'NEG'), ('loading', 'lama banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D259" t="inlineStr">
@@ -5621,7 +5621,7 @@
       </c>
       <c r="C260" t="inlineStr">
         <is>
-          <t>[('cek', 'ga bisa cek', 'NEG')]</t>
+          <t>[('cek pajak kendaraan', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D260" t="inlineStr">
@@ -5641,7 +5641,7 @@
       </c>
       <c r="C261" t="inlineStr">
         <is>
-          <t>[('sertifikat', 'gak bisa di', 'NEG'), ('download', 'gak bisa di', 'NEG')]</t>
+          <t>[('sertifikat vaksin', 'gak bisa', 'NEG'), ('download', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D261" t="inlineStr">
@@ -5661,7 +5661,7 @@
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak bisa digunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'cukup lengkap ', 'POS'), ('aplikasi', 'sangat bermanfaat bagi', 'POS')]</t>
+          <t>[('aplikasi', 'cukup lengkap', 'POS'), ('aplikasi', 'sangat bermanfaat', 'POS')]</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
@@ -5701,7 +5701,7 @@
       </c>
       <c r="C264" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'parah dimana', 'NEG'), ('pelayanannya', 'parah pelayanannya', 'NEG')]</t>
+          <t>[('pelayanan', 'parah', 'NEG'), ('pelayanannya', 'parah', 'NEG')]</t>
         </is>
       </c>
       <c r="D264" t="inlineStr">
@@ -5721,7 +5721,7 @@
       </c>
       <c r="C265" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak bisa dipake ', 'NEG')]</t>
+          <t>[('aplikasi', 'gak bisa dipake', 'NEG')]</t>
         </is>
       </c>
       <c r="D265" t="inlineStr">
@@ -5741,7 +5741,7 @@
       </c>
       <c r="C266" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'bagus tetapi', 'NEG'), ('aplikasinya', 'sering error ', 'NEG')]</t>
+          <t>[('aplikasinya', 'bagus', 'NEG'), ('aplikasinya', 'sering error', 'NEG')]</t>
         </is>
       </c>
       <c r="D266" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>[('ketik', 'gak bisa di', 'NEG'), ('ketik', 'gajelas banget ', 'NEG')]</t>
+          <t>[('ketik', 'gak bisa', 'NEG'), ('ketik', 'gajelas banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>[('akses', 'tidak bisa di', 'NEG')]</t>
+          <t>[('akses', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
@@ -5801,7 +5801,7 @@
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>[('login', 'susah buat', 'NEG')]</t>
+          <t>[('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
@@ -5821,7 +5821,7 @@
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'mempermudah dlm', 'POS'), ('pelayanan', 'mempermudah dlm', 'POS'), ('pelayanan', 'sangat membantu dan', 'POS'), ('digital', 'mempermudah dlm', 'POS')]</t>
+          <t>[('pelayanan masyarakat via digital', 'mempermudah', 'POS'), ('pelayanan masyarakat', 'mempermudah', 'POS'), ('pelayanan masyarakat', 'sangat membantu', 'POS'), ('digital', 'mempermudah', 'POS')]</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="C271" t="inlineStr">
         <is>
-          <t>[('login', 'tidak bisa login', 'NEG')]</t>
+          <t>[('login', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D271" t="inlineStr">
@@ -5861,7 +5861,7 @@
       </c>
       <c r="C272" t="inlineStr">
         <is>
-          <t>[('login', 'gabisa login', 'NEG')]</t>
+          <t>[('login', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D272" t="inlineStr">
@@ -5881,7 +5881,7 @@
       </c>
       <c r="C273" t="inlineStr">
         <is>
-          <t>[('load', 'gajelas load', 'NEG'), ('load', 'lama bgt ', 'NEG')]</t>
+          <t>[('load', 'gajelas', 'NEG'), ('load', 'lama bgt', 'NEG')]</t>
         </is>
       </c>
       <c r="D273" t="inlineStr">
@@ -5901,7 +5901,7 @@
       </c>
       <c r="C274" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sampahh ', 'NEG')]</t>
+          <t>[('aplikasi', 'sampahh', 'NEG')]</t>
         </is>
       </c>
       <c r="D274" t="inlineStr">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'error terus ', 'NEG')]</t>
+          <t>[('aplikasi', 'error terus', 'NEG')]</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="C276" t="inlineStr">
         <is>
-          <t>[('cek', 'susah banget ', 'NEG')]</t>
+          <t>[('cek vaksin', 'susah banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D276" t="inlineStr">
@@ -5961,7 +5961,7 @@
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga mau sama', 'NEG'), ('aplikasi', 'bodoh ga', 'NEG')]</t>
+          <t>[('aplikasi', 'ga mau', 'NEG'), ('aplikasi', 'bodoh', 'NEG')]</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -5981,7 +5981,7 @@
       </c>
       <c r="C278" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'maintenance mulu ', 'NEG')]</t>
+          <t>[('aplikasi', 'maintenance mulu', 'NEG')]</t>
         </is>
       </c>
       <c r="D278" t="inlineStr">
@@ -6001,7 +6001,7 @@
       </c>
       <c r="C279" t="inlineStr">
         <is>
-          <t>[('email', 'tidak d respon2 mind', 'NEG')]</t>
+          <t>[('email', 'tidak d respon2', 'NEG')]</t>
         </is>
       </c>
       <c r="D279" t="inlineStr">
@@ -6021,7 +6021,7 @@
       </c>
       <c r="C280" t="inlineStr">
         <is>
-          <t>[('buka', 'enggak bisa buka', 'NEG')]</t>
+          <t>[('buka', 'enggak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D280" t="inlineStr">
@@ -6041,7 +6041,7 @@
       </c>
       <c r="C281" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'masuk iklan2 ', 'NEG')]</t>
+          <t>[('aplikasi', 'masuk iklan2', 'NEG')]</t>
         </is>
       </c>
       <c r="D281" t="inlineStr">
@@ -6061,7 +6061,7 @@
       </c>
       <c r="C282" t="inlineStr">
         <is>
-          <t>[('responnya', 'lama banget ', 'NEG'), ('respon', 'lama ', 'NEG')]</t>
+          <t>[('responnya', 'lama banget', 'NEG'), ('respon', 'lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D282" t="inlineStr">
@@ -6081,7 +6081,7 @@
       </c>
       <c r="C283" t="inlineStr">
         <is>
-          <t>[('ngecek', 'ngak bisa keluar ', 'NEG')]</t>
+          <t>[('ngecek pelat nomor kanapa', 'ngak bisa keluar', 'NEG')]</t>
         </is>
       </c>
       <c r="D283" t="inlineStr">
@@ -6101,7 +6101,7 @@
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>[('apl', 'jlek ', 'NEG')]</t>
+          <t>[('apl', 'jlek', 'NEG')]</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -6121,7 +6121,7 @@
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>[('respon', 'lama skali ', 'NEG'), ('respon', 'sering gagal pis', 'NEG')]</t>
+          <t>[('respon', 'lama skali', 'NEG'), ('respon', 'sering gagal', 'NEG')]</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="C286" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'berguna bagi', 'POS')]</t>
+          <t>[('aplikasinya', 'berguna', 'POS')]</t>
         </is>
       </c>
       <c r="D286" t="inlineStr">
@@ -6161,7 +6161,7 @@
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>[('scan', 'kacau banget scan', 'NEG'), ('scan', 'gak fungsi ', 'NEG')]</t>
+          <t>[('scan', 'kacau banget', 'NEG'), ('scan', 'gak fungsi', 'NEG')]</t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
@@ -6181,7 +6181,7 @@
       </c>
       <c r="C288" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'buruk saya', 'NEG'), ('login', 'ga bisa tolong', 'NEG'), ('daftar', 'ga bisa karena', 'NEG')]</t>
+          <t>[('aplikasi', 'buruk', 'NEG'), ('login', 'ga bisa', 'NEG'), ('daftar', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D288" t="inlineStr">
@@ -6221,7 +6221,7 @@
       </c>
       <c r="C290" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bodoh ', 'NEG'), ('login', 'tidak bisa login', 'NEG')]</t>
+          <t>[('aplikasi', 'bodoh', 'NEG'), ('login', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D290" t="inlineStr">
@@ -6241,7 +6241,7 @@
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>[('memori', 'menuhin memori', 'NEG')]</t>
+          <t>[('memori', 'menuhin', 'NEG')]</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
@@ -6261,7 +6261,7 @@
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>[('loading', 'lama ', 'NEG')]</t>
+          <t>[('loading', 'lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -6281,7 +6281,7 @@
       </c>
       <c r="C293" t="inlineStr">
         <is>
-          <t>[('input', 'susah amat ', 'NEG')]</t>
+          <t>[('input capchanya', 'susah amat', 'NEG')]</t>
         </is>
       </c>
       <c r="D293" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="C294" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'menyusahkan ', 'NEG'), ('masuk', 'gak bisa masuk', 'NEG')]</t>
+          <t>[('aplikasi', 'menyusahkan', 'NEG'), ('masuk', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D294" t="inlineStr">
@@ -6321,7 +6321,7 @@
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>[('upgrade', 'tambah jelek ', 'NEG')]</t>
+          <t>[('upgrade', 'tambah jelek', 'NEG')]</t>
         </is>
       </c>
       <c r="D295" t="inlineStr">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="C296" t="inlineStr">
         <is>
-          <t>[('dibuka', 'gak bisa dibuka', 'NEG')]</t>
+          <t>[('dibuka', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D296" t="inlineStr">
@@ -6361,7 +6361,7 @@
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>[('sistem', 'kurang terintegrasi dgn', 'NEG')]</t>
+          <t>[('sistem', 'kurang terintegrasi', 'NEG')]</t>
         </is>
       </c>
       <c r="D297" t="inlineStr">
@@ -6381,7 +6381,7 @@
       </c>
       <c r="C298" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat responsif ', 'POS'), ('aplikasi', 'sangat bagus aplikasi', 'NEG')]</t>
+          <t>[('aplikasi', 'sangat responsif', 'POS'), ('aplikasi', 'sangat bagus', 'NEG')]</t>
         </is>
       </c>
       <c r="D298" t="inlineStr">
@@ -6401,7 +6401,7 @@
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>[('proses', 'lama sekali masukan', 'NEG')]</t>
+          <t>[('proses', 'lama sekali', 'NEG')]</t>
         </is>
       </c>
       <c r="D299" t="inlineStr">
@@ -6421,7 +6421,7 @@
       </c>
       <c r="C300" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak dapat dipaham ', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak dapat dipaham', 'NEG')]</t>
         </is>
       </c>
       <c r="D300" t="inlineStr">
@@ -6441,7 +6441,7 @@
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>[('scan', 'lama bangettt scan', 'NEG')]</t>
+          <t>[('scan barcode', 'lama bangettt', 'NEG')]</t>
         </is>
       </c>
       <c r="D301" t="inlineStr">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="C302" t="inlineStr">
         <is>
-          <t>[('bikin', 'susah amat bikin', 'NEG')]</t>
+          <t>[('bikin faswortny', 'susah amat', 'NEG')]</t>
         </is>
       </c>
       <c r="D302" t="inlineStr">
@@ -6481,7 +6481,7 @@
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat bagus membantu', 'POS')]</t>
+          <t>[('aplikasi', 'sangat bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D303" t="inlineStr">
@@ -6501,7 +6501,7 @@
       </c>
       <c r="C304" t="inlineStr">
         <is>
-          <t>[('input', 'ng bisa ', 'NEG'), ('cek', 'belum punya ehac dan', 'NEG')]</t>
+          <t>[('input no otp', 'ng bisa', 'NEG'), ('cek infonyo', 'belum punya ehac', 'NEG')]</t>
         </is>
       </c>
       <c r="D304" t="inlineStr">
@@ -6521,7 +6521,7 @@
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>[('kodenya', 'lama anj', 'NEG')]</t>
+          <t>[('kodenya', 'lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D305" t="inlineStr">
@@ -6541,7 +6541,7 @@
       </c>
       <c r="C306" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'mudah untuk digunakan sekaligus', 'POS'), ('aplikasi', 'sangat cepat dalam', 'POS'), ('pengupload', 'sangat cepat dalam', 'POS')]</t>
+          <t>[('aplikasi', 'mudah untuk digunakan', 'POS'), ('aplikasi', 'sangat cepat', 'POS'), ('pengupload an berkas', 'sangat cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D306" t="inlineStr">
@@ -6561,7 +6561,7 @@
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>[('filter', 'tidak bisa filter', 'NEG'), ('filter', 'tidak bisa filter', 'NEG')]</t>
+          <t>[('filter lokasi', 'tidak bisa', 'NEG'), ('filter', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
@@ -6581,7 +6581,7 @@
       </c>
       <c r="C308" t="inlineStr">
         <is>
-          <t>[('scan', 'ga terdaftar pd', 'NEG'), ('loading', 'terus ', 'NEG')]</t>
+          <t>[('scan', 'ga terdaftar', 'NEG'), ('loading', 'terus', 'NEG')]</t>
         </is>
       </c>
       <c r="D308" t="inlineStr">
@@ -6601,7 +6601,7 @@
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sering eror eror', 'NEG'), ('aplikasi', 'eror terus', 'NEG'), ('aplikasi', 'eror terus', 'NEG')]</t>
+          <t>[('aplikasi', 'sering eror', 'NEG'), ('aplikasi', 'eror', 'NEG'), ('aplikasi', 'eror', 'NEG')]</t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
@@ -6621,7 +6621,7 @@
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sampah begini', 'NEG')]</t>
+          <t>[('aplikasi', 'sampah', 'NEG')]</t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
@@ -6641,7 +6641,7 @@
       </c>
       <c r="C311" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'problematik ', 'NEG'), ('admin', 'di persulit juga', 'NEG')]</t>
+          <t>[('aplikasi', 'problematik', 'NEG'), ('admin apk', 'di persulit', 'NEG')]</t>
         </is>
       </c>
       <c r="D311" t="inlineStr">
@@ -6661,7 +6661,7 @@
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'paling gajelas ', 'NEG')]</t>
+          <t>[('aplikasi', 'paling gajelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
@@ -6681,7 +6681,7 @@
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'susah di buka ', 'NEG'), ('aplikasinya', 'lemot dan', 'NEG')]</t>
+          <t>[('aplikasinya', 'susah di buka', 'NEG'), ('aplikasinya', 'lemot', 'NEG')]</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -6721,7 +6721,7 @@
       </c>
       <c r="C315" t="inlineStr">
         <is>
-          <t>[('helpdesk', 'nggak pernah respon ', 'NEG'), ('data', 'nggak ada ', 'NEG')]</t>
+          <t>[('helpdesk', 'nggak pernah respon', 'NEG'), ('data', 'nggak ada', 'NEG')]</t>
         </is>
       </c>
       <c r="D315" t="inlineStr">
@@ -6741,7 +6741,7 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>[('apk', 'gak bisa apa', 'NEG'), ('check', 'susah ', 'NEG')]</t>
+          <t>[('apk', 'gak bisa', 'NEG'), ('check aja', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>[('berkunjung', 'ribet mau', 'NEG'), ('berkunjung', 'sulit banget ', 'NEG')]</t>
+          <t>[('berkunjung', 'ribet', 'NEG'), ('berkunjung', 'sulit banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
@@ -6781,7 +6781,7 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>[('verifikasi', 'susah verifikasi', 'NEG')]</t>
+          <t>[('verifikasi akun', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
@@ -6801,7 +6801,7 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gk guna sama', 'NEG'), ('aplikasi', 'ganti ini aplikasi . gk guna sama', 'NEG')]</t>
+          <t>[('aplikasi', 'gk guna', 'NEG'), ('aplikasi', 'ganti ini aplikasi . gk guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
@@ -6821,7 +6821,7 @@
       </c>
       <c r="C320" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'butut gab', 'NEG'), ('aplikasi', 'gabisa cek ', 'NEG')]</t>
+          <t>[('aplikasi', 'butut', 'NEG'), ('aplikasi', 'gabisa cek', 'NEG')]</t>
         </is>
       </c>
       <c r="D320" t="inlineStr">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="C321" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'keren banget sih ', 'POS'), ('aplikasi', 'tidak turun ya', 'NEG')]</t>
+          <t>[('aplikasi', 'keren banget sih', 'POS'), ('aplikasi', 'tidak turun', 'NEG')]</t>
         </is>
       </c>
       <c r="D321" t="inlineStr">
@@ -6861,7 +6861,7 @@
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'jelek aplikasinya', 'NEG'), ('aplikasinya', 'gabisaaaa ', 'NEG'), ('customer', 'erorr ', 'NEG')]</t>
+          <t>[('aplikasinya', 'jelek', 'NEG'), ('aplikasinya', 'gabisaaaa', 'NEG'), ('customer servicenya', 'erorr', 'NEG')]</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
@@ -6881,7 +6881,7 @@
       </c>
       <c r="C323" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sering error ', 'NEG'), ('verifikasi', 'gagal ', 'NEG')]</t>
+          <t>[('aplikasi', 'sering error', 'NEG'), ('verifikasi', 'gagal', 'NEG')]</t>
         </is>
       </c>
       <c r="D323" t="inlineStr">
@@ -6901,7 +6901,7 @@
       </c>
       <c r="C324" t="inlineStr">
         <is>
-          <t>[('login', 'gak bisa login', 'NEG')]</t>
+          <t>[('login', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D324" t="inlineStr">
@@ -6921,7 +6921,7 @@
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>[('login', 'tidak bisa login', 'NEG')]</t>
+          <t>[('login', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
@@ -6941,7 +6941,7 @@
       </c>
       <c r="C326" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bagus banget lho', 'POS'), ('search', 'segera diperbaiki ', 'NEG'), ('search', 'bermasalah ', 'NEG')]</t>
+          <t>[('aplikasi', 'bagus banget', 'POS'), ('search engine', 'segera diperbaiki', 'NEG'), ('search engine', 'bermasalah', 'NEG')]</t>
         </is>
       </c>
       <c r="D326" t="inlineStr">
@@ -6961,7 +6961,7 @@
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>[('cek', 'gbs cek', 'NEG')]</t>
+          <t>[('cek info motor', 'gbs', 'NEG')]</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
@@ -6981,7 +6981,7 @@
       </c>
       <c r="C328" t="inlineStr">
         <is>
-          <t>[('respon', 'kurang cepat dan', 'NEG'), ('respon', 'membingungkan karena', 'NEG')]</t>
+          <t>[('respon', 'kurang cepat', 'NEG'), ('respon', 'membingungkan', 'NEG')]</t>
         </is>
       </c>
       <c r="D328" t="inlineStr">
@@ -7021,7 +7021,7 @@
       </c>
       <c r="C330" t="inlineStr">
         <is>
-          <t>[('scan', 'ga bisa ', 'NEG')]</t>
+          <t>[('scan produk', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D330" t="inlineStr">
@@ -7041,7 +7041,7 @@
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>[('pendaftaran', 'tolong perbaiki masalah untuk', 'NEG'), ('daftar', 'gabisa daftar', 'NEG')]</t>
+          <t>[('pendaftaran vaksin', 'tolong perbaiki masalah', 'NEG'), ('daftar', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
@@ -7061,7 +7061,7 @@
       </c>
       <c r="C332" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'mantap ', 'POS')]</t>
+          <t>[('aplikasi', 'mantap', 'POS')]</t>
         </is>
       </c>
       <c r="D332" t="inlineStr">
@@ -7081,7 +7081,7 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>[('dibuka', 'g bisa dibuka', 'NEG')]</t>
+          <t>[('dibuka', 'g bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D333" t="inlineStr">
@@ -7101,7 +7101,7 @@
       </c>
       <c r="C334" t="inlineStr">
         <is>
-          <t>[('apk', 'payah apk', 'NEG'), ('login', 'susah ', 'NEG')]</t>
+          <t>[('apk', 'payah', 'NEG'), ('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D334" t="inlineStr">
@@ -7141,7 +7141,7 @@
       </c>
       <c r="C336" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'tolong segera diperbaiki aplikasinya', 'NEG'), ('aplikasinya', 'segera diperbaiki aplikasinya', 'NEG')]</t>
+          <t>[('aplikasinya', 'tolong segera diperbaiki', 'NEG'), ('aplikasinya', 'segera diperbaiki', 'NEG')]</t>
         </is>
       </c>
       <c r="D336" t="inlineStr">
@@ -7161,7 +7161,7 @@
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>[('update', 'tidak berguna ', 'NEG'), ('update', 'lengkap dan', 'POS'), ('fitur', 'lengkap dan', 'POS')]</t>
+          <t>[('update', 'tidak berguna', 'NEG'), ('update fitur', 'lengkap', 'POS'), ('fitur', 'lengkap', 'POS')]</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
@@ -7181,7 +7181,7 @@
       </c>
       <c r="C338" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak jelas ', 'NEG')]</t>
+          <t>[('aplikasi', 'gak jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D338" t="inlineStr">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="C339" t="inlineStr">
         <is>
-          <t>[('perbaikan', 'ga ada perbaikan', 'NEG')]</t>
+          <t>[('perbaikan', 'ga ada', 'NEG')]</t>
         </is>
       </c>
       <c r="D339" t="inlineStr">
@@ -7221,7 +7221,7 @@
       </c>
       <c r="C340" t="inlineStr">
         <is>
-          <t>[('laporan', 'cepat di tindak lanjuti dan', 'POS')]</t>
+          <t>[('laporan', 'cepat di tindak lanjuti', 'POS')]</t>
         </is>
       </c>
       <c r="D340" t="inlineStr">
@@ -7241,7 +7241,7 @@
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>[('appnya', 'bapuk ', 'NEG')]</t>
+          <t>[('appnya', 'bapuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
@@ -7261,7 +7261,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>[('lihat', 'gak bisa ', 'NEG')]</t>
+          <t>[('lihat pajek bangunan', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
@@ -7281,7 +7281,7 @@
       </c>
       <c r="C343" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat bagus sangat', 'POS')]</t>
+          <t>[('aplikasi', 'sangat bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D343" t="inlineStr">
@@ -7301,7 +7301,7 @@
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>[('cari', 'gak bisa cari', 'NEG')]</t>
+          <t>[('cari lokasi', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
@@ -7321,7 +7321,7 @@
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak bisa update', 'NEG'), ('aplikasi', 'gak bisa update aplikasi', 'NEG'), ('update', 'gak bisa update', 'NEG'), ('update', 'gak bisa update aplikasi', 'NEG')]</t>
+          <t>[('aplikasi', 'gak bisa', 'NEG'), ('aplikasi', 'gak bisa update', 'NEG'), ('update aplikasi', 'gak bisa', 'NEG'), ('update aplikasi', 'gak bisa update', 'NEG')]</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
@@ -7341,7 +7341,7 @@
       </c>
       <c r="C346" t="inlineStr">
         <is>
-          <t>[('developernya', 'banyak bug dm', 'NEG')]</t>
+          <t>[('developernya', 'banyak bug', 'NEG')]</t>
         </is>
       </c>
       <c r="D346" t="inlineStr">
@@ -7361,7 +7361,7 @@
       </c>
       <c r="C347" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga beres ', 'NEG'), ('aplikasi', 'ga bisa di gunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'ga beres', 'NEG'), ('aplikasi', 'ga bisa di gunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D347" t="inlineStr">
@@ -7381,7 +7381,7 @@
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>[('fiktur', 'lumayan ', 'NEG'), ('lapor', 'lumayan ', 'NEG')]</t>
+          <t>[('fiktur lapor', 'lumayan', 'NEG'), ('lapor', 'lumayan', 'NEG')]</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
@@ -7401,7 +7401,7 @@
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>[('login', 'susah untuk', 'NEG')]</t>
+          <t>[('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
@@ -7421,7 +7421,7 @@
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>[('error', 'banyak error', 'NEG')]</t>
+          <t>[('error', 'banyak', 'NEG')]</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="C351" t="inlineStr">
         <is>
-          <t>[('ngecek', 'ga bisa bisa', 'NEG')]</t>
+          <t>[('ngecek', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D351" t="inlineStr">
@@ -7461,7 +7461,7 @@
       </c>
       <c r="C352" t="inlineStr">
         <is>
-          <t>[('loading', 'sangat lama saat', 'NEG'), ('masuk', 'sangat lama saat', 'NEG'), ('loading', 'sangat lama saat', 'NEG')]</t>
+          <t>[('loading masuk', 'sangat lama', 'NEG'), ('masuk', 'sangat lama', 'NEG'), ('loading', 'sangat lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D352" t="inlineStr">
@@ -7481,7 +7481,7 @@
       </c>
       <c r="C353" t="inlineStr">
         <is>
-          <t>[('loading', 'lama mana', 'NEG'), ('scan', 'ga pernah sbntr dan', 'NEG')]</t>
+          <t>[('loading', 'lama', 'NEG'), ('scan', 'ga pernah sbntr', 'NEG')]</t>
         </is>
       </c>
       <c r="D353" t="inlineStr">
@@ -7501,7 +7501,7 @@
       </c>
       <c r="C354" t="inlineStr">
         <is>
-          <t>[('verfikasi', 'ga bisa ver', 'NEG'), ('aplikasi', 'gak jelas banyak', 'NEG'), ('aplikasi', 'banyak kesulitan login maupun', 'NEG')]</t>
+          <t>[('verfikasi', 'ga bisa', 'NEG'), ('aplikasi', 'gak jelas', 'NEG'), ('aplikasi', 'banyak kesulitan login', 'NEG')]</t>
         </is>
       </c>
       <c r="D354" t="inlineStr">
@@ -7521,7 +7521,7 @@
       </c>
       <c r="C355" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat bagus ', 'POS')]</t>
+          <t>[('aplikasi', 'sangat bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D355" t="inlineStr">
@@ -7541,7 +7541,7 @@
       </c>
       <c r="C356" t="inlineStr">
         <is>
-          <t>[('ngecek', 'ngga bisa buat', 'NEG')]</t>
+          <t>[('ngecek', 'ngga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D356" t="inlineStr">
@@ -7561,7 +7561,7 @@
       </c>
       <c r="C357" t="inlineStr">
         <is>
-          <t>[('masuk', 'gajelas ga', 'NEG'), ('masuk', 'ga bisa masuk', 'NEG')]</t>
+          <t>[('masuk', 'gajelas', 'NEG'), ('masuk', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D357" t="inlineStr">
@@ -7581,7 +7581,7 @@
       </c>
       <c r="C358" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sampah kek', 'NEG'), ('aplikasi', 'ga kebuka buka', 'NEG')]</t>
+          <t>[('aplikasi', 'sampah', 'NEG'), ('aplikasi', 'ga kebuka', 'NEG')]</t>
         </is>
       </c>
       <c r="D358" t="inlineStr">
@@ -7601,7 +7601,7 @@
       </c>
       <c r="C359" t="inlineStr">
         <is>
-          <t>[('ngescan', 'gabisa nges', 'NEG')]</t>
+          <t>[('ngescan', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D359" t="inlineStr">
@@ -7621,7 +7621,7 @@
       </c>
       <c r="C360" t="inlineStr">
         <is>
-          <t>[('cek', 'gagal mulu padahal', 'NEG'), ('aplikasi', 'jelek bangt sih', 'NEG')]</t>
+          <t>[('cek', 'gagal mulu', 'NEG'), ('aplikasi', 'jelek bangt', 'NEG')]</t>
         </is>
       </c>
       <c r="D360" t="inlineStr">
@@ -7641,7 +7641,7 @@
       </c>
       <c r="C361" t="inlineStr">
         <is>
-          <t>[('app', 'gk bisa dipake ya', 'NEG')]</t>
+          <t>[('app', 'gk bisa dipake', 'NEG')]</t>
         </is>
       </c>
       <c r="D361" t="inlineStr">
@@ -7661,7 +7661,7 @@
       </c>
       <c r="C362" t="inlineStr">
         <is>
-          <t>[('error', 'sering error', 'NEG'), ('error', 'lambat sering', 'NEG')]</t>
+          <t>[('error', 'sering', 'NEG'), ('error', 'lambat', 'NEG')]</t>
         </is>
       </c>
       <c r="D362" t="inlineStr">
@@ -7681,7 +7681,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>[('download', 'lama di', 'NEG')]</t>
+          <t>[('download', 'lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D363" t="inlineStr">
@@ -7701,7 +7701,7 @@
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>[('download', 'gk bisa download', 'NEG')]</t>
+          <t>[('download sertifikat', 'gk bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D364" t="inlineStr">
@@ -7721,7 +7721,7 @@
       </c>
       <c r="C365" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'ga jelas customer', 'NEG'), ('helpdesk', 'gk ada gunanya sama', 'NEG'), ('helpdesk', 'jelek help', 'NEG')]</t>
+          <t>[('aplikasi', 'ga jelas', 'NEG'), ('helpdesk', 'gk ada gunanya', 'NEG'), ('helpdesk', 'jelek', 'NEG')]</t>
         </is>
       </c>
       <c r="D365" t="inlineStr">
@@ -7741,7 +7741,7 @@
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>[('apk', 'gak bisa digunakan lagi', 'NEG')]</t>
+          <t>[('apk', 'gak bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
@@ -7761,7 +7761,7 @@
       </c>
       <c r="C367" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'sangat membantu masyarakat', 'POS'), ('petugasnya', 'ramah ', 'POS')]</t>
+          <t>[('aplikasinya', 'sangat membantu', 'POS'), ('petugasnya', 'ramah', 'POS')]</t>
         </is>
       </c>
       <c r="D367" t="inlineStr">
@@ -7781,7 +7781,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'top bgt ', 'POS'), ('aplikasinya', 'sangat membantu masyarakat', 'POS')]</t>
+          <t>[('aplikasinya', 'top bgt', 'POS'), ('aplikasinya', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D368" t="inlineStr">
@@ -7801,7 +7801,7 @@
       </c>
       <c r="C369" t="inlineStr">
         <is>
-          <t>[('tindak', 'sangat2 lambat ', 'NEG'), ('action', 'sangat2 lambat ', 'NEG')]</t>
+          <t>[('tindak lanjutnya', 'sangat2 lambat', 'NEG'), ('action tindak lanjutnya', 'sangat2 lambat', 'NEG')]</t>
         </is>
       </c>
       <c r="D369" t="inlineStr">
@@ -7821,7 +7821,7 @@
       </c>
       <c r="C370" t="inlineStr">
         <is>
-          <t>[('akses', 'belum bisa akses', 'NEG')]</t>
+          <t>[('akses', 'belum bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D370" t="inlineStr">
@@ -7841,7 +7841,7 @@
       </c>
       <c r="C371" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tolol ', 'NEG'), ('aplikasi', 'gak guna ', 'NEG')]</t>
+          <t>[('aplikasi', 'tolol', 'NEG'), ('aplikasi', 'gak guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D371" t="inlineStr">
@@ -7881,7 +7881,7 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>[('download', 'tidak bisa dibuka mengapa', 'NEG')]</t>
+          <t>[('download', 'tidak bisa dibuka', 'NEG')]</t>
         </is>
       </c>
       <c r="D373" t="inlineStr">
@@ -7901,7 +7901,7 @@
       </c>
       <c r="C374" t="inlineStr">
         <is>
-          <t>[('bug', 'masih banyak bug', 'NEG')]</t>
+          <t>[('bug', 'masih banyak', 'NEG')]</t>
         </is>
       </c>
       <c r="D374" t="inlineStr">
@@ -7921,7 +7921,7 @@
       </c>
       <c r="C375" t="inlineStr">
         <is>
-          <t>[('donlod', 'gk bisa ', 'NEG')]</t>
+          <t>[('donlod', 'gk bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D375" t="inlineStr">
@@ -7941,7 +7941,7 @@
       </c>
       <c r="C376" t="inlineStr">
         <is>
-          <t>[('aksesnya', 'cepat akses', 'POS')]</t>
+          <t>[('aksesnya', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D376" t="inlineStr">
@@ -7981,7 +7981,7 @@
       </c>
       <c r="C378" t="inlineStr">
         <is>
-          <t>[('apk', 'bagus cuma', 'POS')]</t>
+          <t>[('apk', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D378" t="inlineStr">
@@ -8001,7 +8001,7 @@
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>[('daftar', 'error pd', 'NEG')]</t>
+          <t>[('daftar', 'error', 'NEG')]</t>
         </is>
       </c>
       <c r="D379" t="inlineStr">
@@ -8021,7 +8021,7 @@
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat membantu dan', 'POS')]</t>
+          <t>[('aplikasi', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
@@ -8041,7 +8041,7 @@
       </c>
       <c r="C381" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'memudahkan kinerja pegawai dan', 'POS'), ('aplikasi', 'sering ada kendala pada', 'POS')]</t>
+          <t>[('aplikasi', 'memudahkan kinerja pegawai', 'POS'), ('aplikasi', 'sering ada kendala', 'POS')]</t>
         </is>
       </c>
       <c r="D381" t="inlineStr">
@@ -8081,7 +8081,7 @@
       </c>
       <c r="C383" t="inlineStr">
         <is>
-          <t>[('apk', 'tidak mampu mengenali ', 'NEG'), ('apk', 'tidak mampu mengenali ', 'NEG')]</t>
+          <t>[('apk', 'tidak mampu mengenali', 'NEG'), ('apk nya', 'tidak mampu mengenali', 'NEG')]</t>
         </is>
       </c>
       <c r="D383" t="inlineStr">
@@ -8101,7 +8101,7 @@
       </c>
       <c r="C384" t="inlineStr">
         <is>
-          <t>[('apk', 'ngk bisa udh', 'NEG')]</t>
+          <t>[('apk', 'ngk bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D384" t="inlineStr">
@@ -8121,7 +8121,7 @@
       </c>
       <c r="C385" t="inlineStr">
         <is>
-          <t>[('server', 'tidak bisa terhubung ke', 'NEG')]</t>
+          <t>[('server', 'tidak bisa terhubung', 'NEG')]</t>
         </is>
       </c>
       <c r="D385" t="inlineStr">
@@ -8141,7 +8141,7 @@
       </c>
       <c r="C386" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat membantu sekali', 'POS'), ('aplikasi', 'sangat membantu sekali untuk', 'POS'), ('pengurusan', 'sangat membantu sekali', 'POS'), ('pengurusan', 'sangat membantu sekali untuk', 'POS')]</t>
+          <t>[('aplikasi', 'sangat membantu', 'POS'), ('aplikasi', 'sangat membantu sekali', 'POS'), ('pengurusan surat', 'sangat membantu', 'POS'), ('pengurusan surat', 'sangat membantu sekali', 'POS')]</t>
         </is>
       </c>
       <c r="D386" t="inlineStr">
@@ -8161,7 +8161,7 @@
       </c>
       <c r="C387" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'jembot tdk', 'NEG'), ('aplikasi', 'tdk bisa digunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'jembot', 'NEG'), ('aplikasi', 'tdk bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D387" t="inlineStr">
@@ -8181,7 +8181,7 @@
       </c>
       <c r="C388" t="inlineStr">
         <is>
-          <t>[('versi', 'tidak jelas ', 'NEG')]</t>
+          <t>[('versi terbaru', 'tidak jelas', 'NEG')]</t>
         </is>
       </c>
       <c r="D388" t="inlineStr">
@@ -8201,7 +8201,7 @@
       </c>
       <c r="C389" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak guna gak', 'NEG'), ('login', 'gabisa login', 'NEG')]</t>
+          <t>[('aplikasi', 'gak guna', 'NEG'), ('login', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D389" t="inlineStr">
@@ -8241,7 +8241,7 @@
       </c>
       <c r="C391" t="inlineStr">
         <is>
-          <t>[('loading', 'full loading', 'POS')]</t>
+          <t>[('loading', 'full', 'POS')]</t>
         </is>
       </c>
       <c r="D391" t="inlineStr">
@@ -8261,7 +8261,7 @@
       </c>
       <c r="C392" t="inlineStr">
         <is>
-          <t>[('antre', 'susah bgt ya', 'NEG')]</t>
+          <t>[('antre faskes', 'susah bgt', 'NEG')]</t>
         </is>
       </c>
       <c r="D392" t="inlineStr">
@@ -8281,7 +8281,7 @@
       </c>
       <c r="C393" t="inlineStr">
         <is>
-          <t>[('login', 'ngga bisa login', 'NEG')]</t>
+          <t>[('login', 'ngga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D393" t="inlineStr">
@@ -8301,7 +8301,7 @@
       </c>
       <c r="C394" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak guna banyak', 'NEG')]</t>
+          <t>[('aplikasi', 'gak guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D394" t="inlineStr">
@@ -8321,7 +8321,7 @@
       </c>
       <c r="C395" t="inlineStr">
         <is>
-          <t>[('update', 'susahhhhhhhh ', 'NEG')]</t>
+          <t>[('update', 'susahhhhhhhh', 'NEG')]</t>
         </is>
       </c>
       <c r="D395" t="inlineStr">
@@ -8341,7 +8341,7 @@
       </c>
       <c r="C396" t="inlineStr">
         <is>
-          <t>[('update', 'gak bisa dipakai ', 'NEG'), ('update', 'lemot gak', 'NEG')]</t>
+          <t>[('update', 'gak bisa dipakai', 'NEG'), ('update', 'lemot', 'NEG')]</t>
         </is>
       </c>
       <c r="D396" t="inlineStr">
@@ -8361,7 +8361,7 @@
       </c>
       <c r="C397" t="inlineStr">
         <is>
-          <t>[('scan', 'terlalu banyak eror dan', 'NEG'), ('scan', 'tidak bisa mendeteksi produk ', 'NEG'), ('aplikasinya', 'konyol sudah', 'NEG'), ('aplikasinya', 'terlalu banyak eror dan', 'NEG'), ('aplikasinya', 'tidak bisa mendeteksi produk ', 'NEG'), ('aplikasinya', 'lag ', 'NEG')]</t>
+          <t>[('scan', 'terlalu banyak eror', 'NEG'), ('scan', 'tidak bisa mendeteksi produk', 'NEG'), ('aplikasinya', 'konyol', 'NEG'), ('aplikasinya', 'terlalu banyak eror', 'NEG'), ('aplikasinya', 'tidak bisa mendeteksi produk', 'NEG'), ('aplikasinya', 'lag', 'NEG')]</t>
         </is>
       </c>
       <c r="D397" t="inlineStr">
@@ -8381,7 +8381,7 @@
       </c>
       <c r="C398" t="inlineStr">
         <is>
-          <t>[('masuk', 'tidak bisa masuk', 'NEG')]</t>
+          <t>[('masuk', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D398" t="inlineStr">
@@ -8401,7 +8401,7 @@
       </c>
       <c r="C399" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat lengkap &amp;', 'POS'), ('aplikasi', 'mudah digunakan oleh', 'POS')]</t>
+          <t>[('aplikasi', 'sangat lengkap', 'POS'), ('aplikasi', 'mudah digunakan', 'POS')]</t>
         </is>
       </c>
       <c r="D399" t="inlineStr">
@@ -8421,7 +8421,7 @@
       </c>
       <c r="C400" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lemot ', 'NEG'), ('aplikasi', 'low respon ', 'NEG')]</t>
+          <t>[('aplikasi', 'lemot', 'NEG'), ('aplikasi', 'low respon', 'NEG')]</t>
         </is>
       </c>
       <c r="D400" t="inlineStr">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="C401" t="inlineStr">
         <is>
-          <t>[('login', 'ga bisa login', 'NEG')]</t>
+          <t>[('login', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D401" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="C402" t="inlineStr">
         <is>
-          <t>[('hasil', 'tdk langsung keluar ', 'NEG')]</t>
+          <t>[('hasil scan', 'tdk langsung keluar', 'NEG')]</t>
         </is>
       </c>
       <c r="D402" t="inlineStr">
@@ -8481,7 +8481,7 @@
       </c>
       <c r="C403" t="inlineStr">
         <is>
-          <t>[('daftar', 'ga bisa daftar', 'NEG')]</t>
+          <t>[('daftar', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D403" t="inlineStr">
@@ -8501,7 +8501,7 @@
       </c>
       <c r="C404" t="inlineStr">
         <is>
-          <t>[('login', 'gak bisa ', 'NEG'), ('help', 'gak bisa ', 'NEG'), ('login', 'gak bisa ', 'NEG')]</t>
+          <t>[('login', 'gak bisa', 'NEG'), ('help desk', 'gak bisa', 'NEG'), ('login nomor', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D404" t="inlineStr">
@@ -8521,7 +8521,7 @@
       </c>
       <c r="C405" t="inlineStr">
         <is>
-          <t>[('apk', 'sangat membantu untuk', 'POS')]</t>
+          <t>[('apk', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D405" t="inlineStr">
@@ -8561,7 +8561,7 @@
       </c>
       <c r="C407" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak berguna ', 'NEG')]</t>
+          <t>[('aplikasi', 'gak berguna', 'NEG')]</t>
         </is>
       </c>
       <c r="D407" t="inlineStr">
@@ -8581,7 +8581,7 @@
       </c>
       <c r="C408" t="inlineStr">
         <is>
-          <t>[('login', 'gakbisa ', 'NEG')]</t>
+          <t>[('login', 'gakbisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D408" t="inlineStr">
@@ -8621,7 +8621,7 @@
       </c>
       <c r="C410" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'gk bs ', 'NEG')]</t>
+          <t>[('aplikasinya', 'gk bs', 'NEG')]</t>
         </is>
       </c>
       <c r="D410" t="inlineStr">
@@ -8641,7 +8641,7 @@
       </c>
       <c r="C411" t="inlineStr">
         <is>
-          <t>[('scan', 'loading setengah tahun ', 'NEG'), ('aplikasi', 'lemot ', 'NEG')]</t>
+          <t>[('scan', 'loading setengah tahun', 'NEG'), ('aplikasi', 'lemot', 'NEG')]</t>
         </is>
       </c>
       <c r="D411" t="inlineStr">
@@ -8661,7 +8661,7 @@
       </c>
       <c r="C412" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'bagus ', 'POS'), ('prosesnya', 'cepat ', 'POS')]</t>
+          <t>[('pelayanan', 'bagus', 'POS'), ('prosesnya', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D412" t="inlineStr">
@@ -8681,7 +8681,7 @@
       </c>
       <c r="C413" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lama lebih', 'NEG'), ('aplikasinya', 'tidak bisa d gunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'lama', 'NEG'), ('aplikasinya', 'tidak bisa d gunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D413" t="inlineStr">
@@ -8701,7 +8701,7 @@
       </c>
       <c r="C414" t="inlineStr">
         <is>
-          <t>[('pengambilan', 'kurang dari setengah hari dan', 'NEG')]</t>
+          <t>[('pengambilan dokumen', 'kurang dari setengah hari', 'NEG')]</t>
         </is>
       </c>
       <c r="D414" t="inlineStr">
@@ -8721,7 +8721,7 @@
       </c>
       <c r="C415" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'gak bisa scan sama', 'NEG'), ('aplikasi', 'gak bisa ', 'NEG')]</t>
+          <t>[('aplikasinya', 'gak bisa scan', 'NEG'), ('aplikasi', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D415" t="inlineStr">
@@ -8741,7 +8741,7 @@
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>[('update', 'hilang ', 'NEG')]</t>
+          <t>[('update', 'hilang', 'NEG')]</t>
         </is>
       </c>
       <c r="D416" t="inlineStr">
@@ -8761,7 +8761,7 @@
       </c>
       <c r="C417" t="inlineStr">
         <is>
-          <t>[('bug', 'banyak bug', 'NEG')]</t>
+          <t>[('bug', 'banyak', 'NEG')]</t>
         </is>
       </c>
       <c r="D417" t="inlineStr">
@@ -8781,7 +8781,7 @@
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>[('scan', 'langsung muncul ', 'POS')]</t>
+          <t>[('scan', 'langsung muncul', 'POS')]</t>
         </is>
       </c>
       <c r="D418" t="inlineStr">
@@ -8821,7 +8821,7 @@
       </c>
       <c r="C420" t="inlineStr">
         <is>
-          <t>[('trouble', 'sering tro', 'NEG')]</t>
+          <t>[('trouble', 'sering', 'NEG')]</t>
         </is>
       </c>
       <c r="D420" t="inlineStr">
@@ -8841,7 +8841,7 @@
       </c>
       <c r="C421" t="inlineStr">
         <is>
-          <t>[('login', 'tidak bisa digunakan hanya', 'NEG')]</t>
+          <t>[('login', 'tidak bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D421" t="inlineStr">
@@ -8881,7 +8881,7 @@
       </c>
       <c r="C423" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'hilang data', 'NEG'), ('aplikasi', 'sampah ', 'NEG')]</t>
+          <t>[('aplikasi', 'hilang', 'NEG'), ('aplikasi', 'sampah', 'NEG')]</t>
         </is>
       </c>
       <c r="D423" t="inlineStr">
@@ -8901,7 +8901,7 @@
       </c>
       <c r="C424" t="inlineStr">
         <is>
-          <t>[('membuat', 'tidak tersedia ', 'NEG')]</t>
+          <t>[('membuat akun', 'tidak tersedia', 'NEG')]</t>
         </is>
       </c>
       <c r="D424" t="inlineStr">
@@ -8921,7 +8921,7 @@
       </c>
       <c r="C425" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lemot parah', 'NEG'), ('aplikasi', 'ga guna lemot', 'NEG')]</t>
+          <t>[('aplikasi', 'lemot', 'NEG'), ('aplikasi', 'ga guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D425" t="inlineStr">
@@ -8941,7 +8941,7 @@
       </c>
       <c r="C426" t="inlineStr">
         <is>
-          <t>[('pemulihan', 'gak bisa ', 'NEG')]</t>
+          <t>[('pemulihan akun', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D426" t="inlineStr">
@@ -8981,7 +8981,7 @@
       </c>
       <c r="C428" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'error ya', 'NEG')]</t>
+          <t>[('aplikasi', 'error', 'NEG')]</t>
         </is>
       </c>
       <c r="D428" t="inlineStr">
@@ -9001,7 +9001,7 @@
       </c>
       <c r="C429" t="inlineStr">
         <is>
-          <t>[('update', 'gak bisa di pake ', 'NEG'), ('login', 'kacau mau', 'NEG')]</t>
+          <t>[('update', 'gak bisa di pake', 'NEG'), ('login', 'kacau', 'NEG')]</t>
         </is>
       </c>
       <c r="D429" t="inlineStr">
@@ -9021,7 +9021,7 @@
       </c>
       <c r="C430" t="inlineStr">
         <is>
-          <t>[('user', 'friendly user ', 'POS'), ('pelayanan', 'memudahkan pelayanan', 'POS')]</t>
+          <t>[('user interface', 'friendly user', 'POS'), ('pelayanan', 'memudahkan', 'POS')]</t>
         </is>
       </c>
       <c r="D430" t="inlineStr">
@@ -9041,7 +9041,7 @@
       </c>
       <c r="C431" t="inlineStr">
         <is>
-          <t>[('informasi', 'minim informasi', 'POS')]</t>
+          <t>[('informasi', 'minim', 'POS')]</t>
         </is>
       </c>
       <c r="D431" t="inlineStr">
@@ -9061,7 +9061,7 @@
       </c>
       <c r="C432" t="inlineStr">
         <is>
-          <t>[('apk', 'di kembangkan lagi yaa', 'NEG'), ('apk', 'mohon di perbaiki dan', 'NEG')]</t>
+          <t>[('apk', 'di kembangkan lagi', 'NEG'), ('apk', 'mohon di perbaiki', 'NEG')]</t>
         </is>
       </c>
       <c r="D432" t="inlineStr">
@@ -9081,7 +9081,7 @@
       </c>
       <c r="C433" t="inlineStr">
         <is>
-          <t>[('aplikasih', 'gak membantu sama', 'NEG'), ('helpdesk', 'lambat merespon dan', 'NEG'), ('helpdesk', 'gak membantu menyelesaikan', 'NEG'), ('helpdesk', 'gak membantu menyelesaikan', 'NEG')]</t>
+          <t>[('aplikasih', 'gak membantu', 'NEG'), ('helpdesk kemenkes', 'lambat merespon', 'NEG'), ('helpdesk kemenkes', 'gak membantu', 'NEG'), ('helpdesk', 'gak membantu', 'NEG')]</t>
         </is>
       </c>
       <c r="D433" t="inlineStr">
@@ -9101,7 +9101,7 @@
       </c>
       <c r="C434" t="inlineStr">
         <is>
-          <t>[('scan', 'tidak bisa scan', 'NEG')]</t>
+          <t>[('scan qr code', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D434" t="inlineStr">
@@ -9121,7 +9121,7 @@
       </c>
       <c r="C435" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'abal abal ', 'NEG'), ('aplikasi', 'gk bisa digunakan ', 'NEG')]</t>
+          <t>[('aplikasi', 'abal abal', 'NEG'), ('aplikasi', 'gk bisa digunakan', 'NEG')]</t>
         </is>
       </c>
       <c r="D435" t="inlineStr">
@@ -9141,7 +9141,7 @@
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>[('proses', 'cepat ', 'POS')]</t>
+          <t>[('proses', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D436" t="inlineStr">
@@ -9161,7 +9161,7 @@
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>[('cek', 'tidak bisa cek', 'NEG')]</t>
+          <t>[('cek pajak mobil', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
@@ -9181,7 +9181,7 @@
       </c>
       <c r="C438" t="inlineStr">
         <is>
-          <t>[('apk', 'semakin dimudahkan dengan', 'POS')]</t>
+          <t>[('apk', 'semakin dimudahkan', 'POS')]</t>
         </is>
       </c>
       <c r="D438" t="inlineStr">
@@ -9201,7 +9201,7 @@
       </c>
       <c r="C439" t="inlineStr">
         <is>
-          <t>[('pakai', 'lemot ketika', 'NEG')]</t>
+          <t>[('pakai', 'lemot', 'NEG')]</t>
         </is>
       </c>
       <c r="D439" t="inlineStr">
@@ -9221,7 +9221,7 @@
       </c>
       <c r="C440" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat jelek banget', 'NEG'), ('login', 'jelek banget apk', 'NEG')]</t>
+          <t>[('aplikasi', 'sangat jelek', 'NEG'), ('login', 'jelek banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D440" t="inlineStr">
@@ -9241,7 +9241,7 @@
       </c>
       <c r="C441" t="inlineStr">
         <is>
-          <t>[('regrestasi', 'lambat ', 'NEG')]</t>
+          <t>[('regrestasi', 'lambat', 'NEG')]</t>
         </is>
       </c>
       <c r="D441" t="inlineStr">
@@ -9261,7 +9261,7 @@
       </c>
       <c r="C442" t="inlineStr">
         <is>
-          <t>[('eror', 'sering eror', 'NEG')]</t>
+          <t>[('eror', 'sering', 'NEG')]</t>
         </is>
       </c>
       <c r="D442" t="inlineStr">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="C443" t="inlineStr">
         <is>
-          <t>[('tombol', 'gak ada isinya ', 'NEG')]</t>
+          <t>[('tombol tombol', 'gak ada isinya', 'NEG')]</t>
         </is>
       </c>
       <c r="D443" t="inlineStr">
@@ -9301,7 +9301,7 @@
       </c>
       <c r="C444" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'kurang sempurna ', 'NEG')]</t>
+          <t>[('aplikasi', 'kurang sempurna', 'NEG')]</t>
         </is>
       </c>
       <c r="D444" t="inlineStr">
@@ -9321,7 +9321,7 @@
       </c>
       <c r="C445" t="inlineStr">
         <is>
-          <t>[('data', 'hilang sehingga', 'NEG'), ('sertifikat', 'tidak ditemukan ', 'NEG')]</t>
+          <t>[('data', 'hilang', 'NEG'), ('sertifikat vaksin', 'tidak ditemukan', 'NEG')]</t>
         </is>
       </c>
       <c r="D445" t="inlineStr">
@@ -9341,7 +9341,7 @@
       </c>
       <c r="C446" t="inlineStr">
         <is>
-          <t>[('mengurus', 'mempermudah kami', 'POS')]</t>
+          <t>[('mengurus surat surat', 'mempermudah', 'POS')]</t>
         </is>
       </c>
       <c r="D446" t="inlineStr">
@@ -9361,7 +9361,7 @@
       </c>
       <c r="C447" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'susah untuk digunakanpel', 'NEG'), ('cetak', 'tidak bisa berjalan ', 'NEG'), ('update', 'susah untuk digunakanpel', 'NEG')]</t>
+          <t>[('aplikasi', 'susah untuk', 'NEG'), ('cetak kode bayar', 'tidak bisa berjalan', 'NEG'), ('update aplikasi', 'susah untuk', 'NEG')]</t>
         </is>
       </c>
       <c r="D447" t="inlineStr">
@@ -9381,7 +9381,7 @@
       </c>
       <c r="C448" t="inlineStr">
         <is>
-          <t>[('scan', 'muter - muter doang ', 'NEG'), ('scan', 'lama bgt muter', 'NEG'), ('scan', 'muter - muter doang ', 'NEG')]</t>
+          <t>[('scan pke barcode', 'muter - muter doang', 'NEG'), ('scan pke barcode', 'lama bgt', 'NEG'), ('scan', 'muter - muter doang', 'NEG')]</t>
         </is>
       </c>
       <c r="D448" t="inlineStr">
@@ -9401,7 +9401,7 @@
       </c>
       <c r="C449" t="inlineStr">
         <is>
-          <t>[('pencet', 'bermasalah malah', 'NEG'), ('aplikasi', 'aneh ', 'NEG')]</t>
+          <t>[('pencet email', 'bermasalah', 'NEG'), ('aplikasi', 'aneh', 'NEG')]</t>
         </is>
       </c>
       <c r="D449" t="inlineStr">
@@ -9421,7 +9421,7 @@
       </c>
       <c r="C450" t="inlineStr">
         <is>
-          <t>[('scan', 'muter - muter lama', 'NEG')]</t>
+          <t>[('scan produk', 'muter - muter', 'NEG')]</t>
         </is>
       </c>
       <c r="D450" t="inlineStr">
@@ -9441,7 +9441,7 @@
       </c>
       <c r="C451" t="inlineStr">
         <is>
-          <t>[('aplikasinya', 'gangguan terus ', 'NEG'), ('aplikasinya', 'bosoook ', 'NEG')]</t>
+          <t>[('aplikasinya', 'gangguan terus', 'NEG'), ('aplikasinya', 'bosoook', 'NEG')]</t>
         </is>
       </c>
       <c r="D451" t="inlineStr">
@@ -9481,7 +9481,7 @@
       </c>
       <c r="C453" t="inlineStr">
         <is>
-          <t>[('login', 'tidak bisa login', 'NEG')]</t>
+          <t>[('login', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D453" t="inlineStr">
@@ -9501,7 +9501,7 @@
       </c>
       <c r="C454" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'semakin buruk ', 'NEG'), ('login', 'susah gagal', 'NEG')]</t>
+          <t>[('aplikasi', 'semakin buruk', 'NEG'), ('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D454" t="inlineStr">
@@ -9541,7 +9541,7 @@
       </c>
       <c r="C456" t="inlineStr">
         <is>
-          <t>[('dibuka', 'tidak bisa dibuka', 'NEG')]</t>
+          <t>[('dibuka', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D456" t="inlineStr">
@@ -9581,7 +9581,7 @@
       </c>
       <c r="C458" t="inlineStr">
         <is>
-          <t>[('app', 'gbisa di pake mah', 'NEG')]</t>
+          <t>[('app', 'gbisa di pake', 'NEG')]</t>
         </is>
       </c>
       <c r="D458" t="inlineStr">
@@ -9601,7 +9601,7 @@
       </c>
       <c r="C459" t="inlineStr">
         <is>
-          <t>[('log', 'susah ', 'NEG')]</t>
+          <t>[('log in', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D459" t="inlineStr">
@@ -9621,7 +9621,7 @@
       </c>
       <c r="C460" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gabisa dipake gangguan', 'NEG')]</t>
+          <t>[('aplikasi', 'gabisa dipake', 'NEG')]</t>
         </is>
       </c>
       <c r="D460" t="inlineStr">
@@ -9641,7 +9641,7 @@
       </c>
       <c r="C461" t="inlineStr">
         <is>
-          <t>[('teridentifikasi', 'gak bisa teri', 'NEG'), ('scan', 'gak bisa dipakai lagi', 'NEG'), ('fitur', 'gak bisa dipakai lagi', 'NEG')]</t>
+          <t>[('teridentifikasi produknya', 'gak bisa', 'NEG'), ('scan qr code', 'gak bisa dipakai', 'NEG'), ('fitur scan qr code', 'gak bisa dipakai', 'NEG')]</t>
         </is>
       </c>
       <c r="D461" t="inlineStr">
@@ -9661,7 +9661,7 @@
       </c>
       <c r="C462" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'blm maksimal jangan', 'NEG'), ('sistem', 'dipersulit sistem', 'NEG')]</t>
+          <t>[('aplikasi', 'blm maksimal', 'NEG'), ('sistem', 'dipersulit', 'NEG')]</t>
         </is>
       </c>
       <c r="D462" t="inlineStr">
@@ -9681,7 +9681,7 @@
       </c>
       <c r="C463" t="inlineStr">
         <is>
-          <t>[('dibuka', 'gak bisa " ', 'NEG')]</t>
+          <t>[('dibuka', 'gak bisa "', 'NEG')]</t>
         </is>
       </c>
       <c r="D463" t="inlineStr">
@@ -9701,7 +9701,7 @@
       </c>
       <c r="C464" t="inlineStr">
         <is>
-          <t>[('apk', 'gk bisa d buka untuk', 'NEG'), ('apk', 'tidak bermutu ', 'NEG')]</t>
+          <t>[('apk', 'gk bisa d buka', 'NEG'), ('apk', 'tidak bermutu', 'NEG')]</t>
         </is>
       </c>
       <c r="D464" t="inlineStr">
@@ -9721,7 +9721,7 @@
       </c>
       <c r="C465" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'sangat cepat dan', 'POS'), ('pelayanan', 'ramah ', 'POS')]</t>
+          <t>[('pelayanan', 'sangat cepat', 'POS'), ('pelayanan', 'ramah', 'POS')]</t>
         </is>
       </c>
       <c r="D465" t="inlineStr">
@@ -9741,7 +9741,7 @@
       </c>
       <c r="C466" t="inlineStr">
         <is>
-          <t>[('apps', 'bapuk banget nih', 'NEG')]</t>
+          <t>[('apps', 'bapuk banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D466" t="inlineStr">
@@ -9761,7 +9761,7 @@
       </c>
       <c r="C467" t="inlineStr">
         <is>
-          <t>[('apk', 'bnyak kurangnya ', 'NEG'), ('apk', 'jelek bnyak', 'NEG')]</t>
+          <t>[('apk', 'bnyak kurangnya', 'NEG'), ('apk', 'jelek', 'NEG')]</t>
         </is>
       </c>
       <c r="D467" t="inlineStr">
@@ -9781,7 +9781,7 @@
       </c>
       <c r="C468" t="inlineStr">
         <is>
-          <t>[('respon', 'sangat cepat sekali respon', 'POS'), ('pelayanany', 'sangat puas ', 'POS')]</t>
+          <t>[('respon', 'sangat cepat sekali', 'POS'), ('pelayanany', 'sangat puas', 'POS')]</t>
         </is>
       </c>
       <c r="D468" t="inlineStr">
@@ -9801,7 +9801,7 @@
       </c>
       <c r="C469" t="inlineStr">
         <is>
-          <t>[('login', 'susah untuk', 'NEG')]</t>
+          <t>[('login', 'susah', 'NEG')]</t>
         </is>
       </c>
       <c r="D469" t="inlineStr">
@@ -9821,7 +9821,7 @@
       </c>
       <c r="C470" t="inlineStr">
         <is>
-          <t>[('lapor', 'tidak bisa klik', 'NEG')]</t>
+          <t>[('lapor', 'tidak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D470" t="inlineStr">
@@ -9841,7 +9841,7 @@
       </c>
       <c r="C471" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gak guna ni', 'NEG')]</t>
+          <t>[('aplikasi', 'gak guna', 'NEG')]</t>
         </is>
       </c>
       <c r="D471" t="inlineStr">
@@ -9861,7 +9861,7 @@
       </c>
       <c r="C472" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bagus bermanfaat', 'POS'), ('aplikasi', 'bermanfaat dan', 'POS')]</t>
+          <t>[('aplikasi', 'bagus', 'POS'), ('aplikasi', 'bermanfaat', 'POS')]</t>
         </is>
       </c>
       <c r="D472" t="inlineStr">
@@ -9881,7 +9881,7 @@
       </c>
       <c r="C473" t="inlineStr">
         <is>
-          <t>[('login', 'gabisa apa', 'NEG')]</t>
+          <t>[('login', 'gabisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D473" t="inlineStr">
@@ -9901,7 +9901,7 @@
       </c>
       <c r="C474" t="inlineStr">
         <is>
-          <t>[('buka', 'gag bisa di', 'NEG')]</t>
+          <t>[('buka', 'gag bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D474" t="inlineStr">
@@ -9921,7 +9921,7 @@
       </c>
       <c r="C475" t="inlineStr">
         <is>
-          <t>[('akses', 'ga bisa akses', 'NEG')]</t>
+          <t>[('akses', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D475" t="inlineStr">
@@ -9941,7 +9941,7 @@
       </c>
       <c r="C476" t="inlineStr">
         <is>
-          <t>[('error', 'sering error', 'NEG')]</t>
+          <t>[('error', 'sering', 'NEG')]</t>
         </is>
       </c>
       <c r="D476" t="inlineStr">
@@ -9961,7 +9961,7 @@
       </c>
       <c r="C477" t="inlineStr">
         <is>
-          <t>[('login', 'sulitnya mau', 'NEG')]</t>
+          <t>[('login', 'sulitnya', 'NEG')]</t>
         </is>
       </c>
       <c r="D477" t="inlineStr">
@@ -9981,7 +9981,7 @@
       </c>
       <c r="C478" t="inlineStr">
         <is>
-          <t>[('loading', 'lama hampir', 'NEG')]</t>
+          <t>[('loading', 'lama', 'NEG')]</t>
         </is>
       </c>
       <c r="D478" t="inlineStr">
@@ -10001,7 +10001,7 @@
       </c>
       <c r="C479" t="inlineStr">
         <is>
-          <t>[('apk', 'lemot banget apk', 'NEG')]</t>
+          <t>[('apk', 'lemot banget', 'NEG')]</t>
         </is>
       </c>
       <c r="D479" t="inlineStr">
@@ -10021,7 +10021,7 @@
       </c>
       <c r="C480" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'error ', 'NEG'), ('masuk', 'gk bisa masuk', 'NEG')]</t>
+          <t>[('aplikasi', 'error', 'NEG'), ('masuk', 'gk bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D480" t="inlineStr">
@@ -10041,7 +10041,7 @@
       </c>
       <c r="C481" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'lemot bgt aplikasi', 'NEG')]</t>
+          <t>[('aplikasi', 'lemot bgt', 'NEG')]</t>
         </is>
       </c>
       <c r="D481" t="inlineStr">
@@ -10061,7 +10061,7 @@
       </c>
       <c r="C482" t="inlineStr">
         <is>
-          <t>[('scand', 'gak terdeteksi ', 'NEG'), ('apk', 'gak guna apk', 'NEG'), ('aplikasi', 'mohon di koreksi lagi aplikasi', 'NEG')]</t>
+          <t>[('scand', 'gak terdeteksi', 'NEG'), ('apk', 'gak guna', 'NEG'), ('aplikasi', 'mohon di koreksi lagi', 'NEG')]</t>
         </is>
       </c>
       <c r="D482" t="inlineStr">
@@ -10081,7 +10081,7 @@
       </c>
       <c r="C483" t="inlineStr">
         <is>
-          <t>[('pinjam', 'gk bisa pinjam', 'NEG')]</t>
+          <t>[('pinjam buku', 'gk bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D483" t="inlineStr">
@@ -10101,7 +10101,7 @@
       </c>
       <c r="C484" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bagus ', 'POS'), ('aplikasi', 'sangat membantu ', 'POS')]</t>
+          <t>[('aplikasi', 'bagus', 'POS'), ('aplikasi', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D484" t="inlineStr">
@@ -10121,7 +10121,7 @@
       </c>
       <c r="C485" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat membantu warga', 'POS')]</t>
+          <t>[('aplikasi', 'sangat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D485" t="inlineStr">
@@ -10141,7 +10141,7 @@
       </c>
       <c r="C486" t="inlineStr">
         <is>
-          <t>[('ambulan', 'sangat membantuu ', 'POS'), ('ambulan', 'gratis untuk', 'POS')]</t>
+          <t>[('ambulan', 'sangat membantuu', 'POS'), ('ambulan', 'gratis', 'POS')]</t>
         </is>
       </c>
       <c r="D486" t="inlineStr">
@@ -10161,7 +10161,7 @@
       </c>
       <c r="C487" t="inlineStr">
         <is>
-          <t>[('penyampaian', 'praktis dalam', 'POS'), ('meresponnya', 'cepat ', 'POS')]</t>
+          <t>[('penyampaian keluhan', 'praktis', 'POS'), ('meresponnya', 'cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D487" t="inlineStr">
@@ -10181,7 +10181,7 @@
       </c>
       <c r="C488" t="inlineStr">
         <is>
-          <t>[('alikasinya', 'gak guna ', 'NEG'), ('aplikasinya', 'gak jelas setelah', 'NEG'), ('aplikasinya', 'tolong diperbaiki aplikasinya', 'NEG'), ('tnbk', 'tidak terdeteksi padahal', 'NEG')]</t>
+          <t>[('alikasinya', 'gak guna', 'NEG'), ('aplikasinya', 'gak jelas', 'NEG'), ('aplikasinya', 'tolong diperbaiki', 'NEG'), ('tnbk', 'tidak terdeteksi', 'NEG')]</t>
         </is>
       </c>
       <c r="D488" t="inlineStr">
@@ -10201,7 +10201,7 @@
       </c>
       <c r="C489" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'tidak ada manfaatnya sed', 'NEG')]</t>
+          <t>[('aplikasi', 'tidak ada manfaatnya', 'NEG')]</t>
         </is>
       </c>
       <c r="D489" t="inlineStr">
@@ -10241,7 +10241,7 @@
       </c>
       <c r="C491" t="inlineStr">
         <is>
-          <t>[('update', 'gak bagus lagi', 'NEG'), ('aplikasinya', 'bagus tapi', 'POS')]</t>
+          <t>[('update', 'gak bagus', 'NEG'), ('aplikasinya', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D491" t="inlineStr">
@@ -10261,7 +10261,7 @@
       </c>
       <c r="C492" t="inlineStr">
         <is>
-          <t>[('pengurusan', 'sangat cepat terimakasih', 'POS')]</t>
+          <t>[('pengurusan', 'sangat cepat', 'POS')]</t>
         </is>
       </c>
       <c r="D492" t="inlineStr">
@@ -10281,7 +10281,7 @@
       </c>
       <c r="C493" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'mudah digunakan ', 'POS')]</t>
+          <t>[('aplikasi', 'mudah digunakan', 'POS')]</t>
         </is>
       </c>
       <c r="D493" t="inlineStr">
@@ -10301,7 +10301,7 @@
       </c>
       <c r="C494" t="inlineStr">
         <is>
-          <t>[('pelayanan', 'sangat puas dan', 'POS'), ('pelayanan', 'baik ', 'POS')]</t>
+          <t>[('pelayanan', 'sangat puas', 'POS'), ('pelayanan', 'baik', 'POS')]</t>
         </is>
       </c>
       <c r="D494" t="inlineStr">
@@ -10341,7 +10341,7 @@
       </c>
       <c r="C496" t="inlineStr">
         <is>
-          <t>[('pinjam', 'tidak bisa di download ', 'NEG')]</t>
+          <t>[('pinjam buku', 'tidak bisa di download', 'NEG')]</t>
         </is>
       </c>
       <c r="D496" t="inlineStr">
@@ -10381,7 +10381,7 @@
       </c>
       <c r="C498" t="inlineStr">
         <is>
-          <t>[('login', 'gak bisa login', 'NEG')]</t>
+          <t>[('login', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D498" t="inlineStr">
@@ -10401,7 +10401,7 @@
       </c>
       <c r="C499" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat berguna ', 'POS')]</t>
+          <t>[('aplikasi', 'sangat berguna', 'POS')]</t>
         </is>
       </c>
       <c r="D499" t="inlineStr">
@@ -10421,7 +10421,7 @@
       </c>
       <c r="C500" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'bagus ', 'POS')]</t>
+          <t>[('aplikasi', 'bagus', 'POS')]</t>
         </is>
       </c>
       <c r="D500" t="inlineStr">
@@ -10441,7 +10441,7 @@
       </c>
       <c r="C501" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'payah ', 'NEG'), ('lapor', 'ribet ', 'NEG')]</t>
+          <t>[('aplikasi', 'payah', 'NEG'), ('lapor foto', 'ribet', 'NEG')]</t>
         </is>
       </c>
       <c r="D501" t="inlineStr">
@@ -10461,7 +10461,7 @@
       </c>
       <c r="C502" t="inlineStr">
         <is>
-          <t>[('server', 'error ', 'NEG')]</t>
+          <t>[('server', 'error', 'NEG')]</t>
         </is>
       </c>
       <c r="D502" t="inlineStr">
@@ -10481,7 +10481,7 @@
       </c>
       <c r="C503" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'sangat amat membantu masyarakat', 'POS')]</t>
+          <t>[('aplikasi', 'sangat amat membantu', 'POS')]</t>
         </is>
       </c>
       <c r="D503" t="inlineStr">
@@ -10521,7 +10521,7 @@
       </c>
       <c r="C505" t="inlineStr">
         <is>
-          <t>[('jakwifi', 'susah di akses dan', 'NEG')]</t>
+          <t>[('jakwifi', 'susah di akses', 'NEG')]</t>
         </is>
       </c>
       <c r="D505" t="inlineStr">
@@ -10541,7 +10541,7 @@
       </c>
       <c r="C506" t="inlineStr">
         <is>
-          <t>[('daftar', 'ga bisa ', 'NEG')]</t>
+          <t>[('daftar vaksin', 'ga bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D506" t="inlineStr">
@@ -10561,7 +10561,7 @@
       </c>
       <c r="C507" t="inlineStr">
         <is>
-          <t>[('institut', 'bobrok takut', 'NEG'), ('institut', 'takut ketahuan ', 'NEG')]</t>
+          <t>[('institut', 'bobrok', 'NEG'), ('institut', 'takut ketahuan', 'NEG')]</t>
         </is>
       </c>
       <c r="D507" t="inlineStr">
@@ -10581,7 +10581,7 @@
       </c>
       <c r="C508" t="inlineStr">
         <is>
-          <t>[('mengidentifikasi', 'lola di', 'NEG')]</t>
+          <t>[('mengidentifikasi', 'lola', 'NEG')]</t>
         </is>
       </c>
       <c r="D508" t="inlineStr">
@@ -10601,7 +10601,7 @@
       </c>
       <c r="C509" t="inlineStr">
         <is>
-          <t>[('perawatan', 'tidak mumpuni di', 'NEG'), ('troble', 'sering tro', 'NEG'), ('kualitas', 'tidak mumpuni di', 'NEG')]</t>
+          <t>[('perawatan', 'tidak mumpuni', 'NEG'), ('troble', 'sering', 'NEG'), ('kualitas sdm untuk pengembangan dan perawatan', 'tidak mumpuni', 'NEG')]</t>
         </is>
       </c>
       <c r="D509" t="inlineStr">
@@ -10621,7 +10621,7 @@
       </c>
       <c r="C510" t="inlineStr">
         <is>
-          <t>[('up', 'gak bisa sama', 'NEG')]</t>
+          <t>[('up', 'gak bisa', 'NEG')]</t>
         </is>
       </c>
       <c r="D510" t="inlineStr">
@@ -10641,7 +10641,7 @@
       </c>
       <c r="C511" t="inlineStr">
         <is>
-          <t>[('aplikasi', 'gk berfungsi gini', 'NEG')]</t>
+          <t>[('aplikasi', 'gk berfungsi', 'NEG')]</t>
         </is>
       </c>
       <c r="D511" t="inlineStr">

</xml_diff>